<commit_message>
Adds direct drive wind turbines
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-PV-perovskite.xlsx
+++ b/premise/data/additional_inventories/lci-PV-perovskite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hahnme_a\PycharmProjects\premise\premise\data\additional_inventories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582C2CAF-E8DA-411E-BBB3-24311CB65E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024DBA9C-8815-4691-81F4-CBF85928FE47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-3615" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PV-perovskite" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2828" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2856" uniqueCount="453">
   <si>
     <t>Database</t>
   </si>
@@ -1386,6 +1386,15 @@
   </si>
   <si>
     <t>stockpiling of anode slime from electrorefining of copper, anode</t>
+  </si>
+  <si>
+    <t>electricity production, photovoltaic, at 0.5 kWp, perovskite-on-silicon tandem</t>
+  </si>
+  <si>
+    <t>electricity, low voltage</t>
+  </si>
+  <si>
+    <t>Data from Table 1. Cells per module: 72 | Gross module are: 2 square meter | Performance. Yield over lifetime: 11500 kWh/per module (each module 2 square meter)</t>
   </si>
 </sst>
 </file>
@@ -1736,10 +1745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H736"/>
+  <dimension ref="A1:H747"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A548" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B576" sqref="B576"/>
+    <sheetView tabSelected="1" topLeftCell="A549" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B558" sqref="B558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11351,2561 +11360,2700 @@
         <v>361</v>
       </c>
     </row>
+    <row r="556" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A556" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B556" s="2" t="s">
+        <v>450</v>
+      </c>
+    </row>
     <row r="557" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A557" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B557" s="2" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="558" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A558" s="5" t="s">
+      <c r="A557" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B558" s="5" t="s">
-        <v>386</v>
+      <c r="B557" s="5" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="558" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A558" t="s">
+        <v>3</v>
+      </c>
+      <c r="B558" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="559" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>3</v>
-      </c>
-      <c r="B559" t="s">
-        <v>92</v>
+        <v>5</v>
+      </c>
+      <c r="B559">
+        <v>1</v>
       </c>
     </row>
     <row r="560" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>5</v>
-      </c>
-      <c r="B560">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="B560" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="561" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B561" t="s">
-        <v>387</v>
+        <v>81</v>
       </c>
     </row>
     <row r="562" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B562" t="s">
-        <v>135</v>
+        <v>16</v>
       </c>
     </row>
     <row r="563" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A563" t="s">
-        <v>8</v>
-      </c>
-      <c r="B563" t="s">
-        <v>16</v>
-      </c>
+      <c r="A563" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B563" s="1"/>
+      <c r="C563" s="1"/>
+      <c r="D563" s="1"/>
+      <c r="E563" s="1"/>
+      <c r="F563" s="1"/>
+      <c r="G563" s="1"/>
     </row>
     <row r="564" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A564" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B564" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C564" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D564" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E564" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F564" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G564" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H564" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="565" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A565" t="str">
+        <f>B556</f>
+        <v>electricity production, photovoltaic, at 0.5 kWp, perovskite-on-silicon tandem</v>
+      </c>
+      <c r="B565" s="3">
+        <f>483538.053104108/483538.053104108</f>
+        <v>1</v>
+      </c>
+      <c r="C565" t="str">
+        <f>B561</f>
+        <v>kilowatt hour</v>
+      </c>
+      <c r="E565" t="str">
+        <f>B558</f>
+        <v>RER</v>
+      </c>
+      <c r="F565" t="s">
+        <v>14</v>
+      </c>
+      <c r="G565" t="str">
+        <f>B560</f>
+        <v>electricity, low voltage</v>
+      </c>
+    </row>
+    <row r="566" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A566" t="s">
+        <v>357</v>
+      </c>
+      <c r="B566" s="4">
+        <f>1/(11500)</f>
+        <v>8.6956521739130441E-5</v>
+      </c>
+      <c r="C566" t="s">
+        <v>7</v>
+      </c>
+      <c r="E566" t="s">
+        <v>92</v>
+      </c>
+      <c r="F566" t="s">
+        <v>77</v>
+      </c>
+      <c r="G566" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="568" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A568" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B568" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="569" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A569" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B569" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="570" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>3</v>
+      </c>
+      <c r="B570" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="571" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>5</v>
+      </c>
+      <c r="B571">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="572" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>6</v>
+      </c>
+      <c r="B572" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="573" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>7</v>
+      </c>
+      <c r="B573" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="574" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>8</v>
+      </c>
+      <c r="B574" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="575" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A575" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B564" s="1"/>
-      <c r="C564" s="1"/>
-      <c r="D564" s="1"/>
-      <c r="E564" s="1"/>
-      <c r="F564" s="1"/>
-      <c r="G564" s="1"/>
-    </row>
-    <row r="565" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A565" s="1" t="s">
+      <c r="B575" s="1"/>
+      <c r="C575" s="1"/>
+      <c r="D575" s="1"/>
+      <c r="E575" s="1"/>
+      <c r="F575" s="1"/>
+      <c r="G575" s="1"/>
+    </row>
+    <row r="576" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A576" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B565" s="1" t="s">
+      <c r="B576" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C565" s="1" t="s">
+      <c r="C576" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D565" s="1" t="s">
+      <c r="D576" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E565" s="1" t="s">
+      <c r="E576" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F565" s="1" t="s">
+      <c r="F576" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G565" s="1" t="s">
+      <c r="G576" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H565" s="1" t="s">
+      <c r="H576" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="566" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A566" t="str">
-        <f>B557</f>
+    <row r="577" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A577" t="str">
+        <f>B568</f>
         <v>exhaust abatement, for perovskite</v>
       </c>
-      <c r="B566" s="3">
+      <c r="B577" s="3">
         <f>-1</f>
         <v>-1</v>
       </c>
-      <c r="C566" t="str">
-        <f>B562</f>
+      <c r="C577" t="str">
+        <f>B573</f>
         <v>cubic meter</v>
       </c>
-      <c r="E566" t="str">
-        <f>B559</f>
+      <c r="E577" t="str">
+        <f>B570</f>
         <v>DE</v>
       </c>
-      <c r="F566" t="s">
+      <c r="F577" t="s">
         <v>14</v>
       </c>
-      <c r="G566" t="str">
-        <f>B561</f>
+      <c r="G577" t="str">
+        <f>B572</f>
         <v>abated exhaust</v>
       </c>
-      <c r="H566" t="s">
+      <c r="H577" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="567" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A567" t="s">
+    <row r="578" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
         <v>106</v>
       </c>
-      <c r="B567">
+      <c r="B578">
         <v>1.6111111111111111E-5</v>
       </c>
-      <c r="C567" t="s">
-        <v>79</v>
-      </c>
-      <c r="E567" t="s">
+      <c r="C578" t="s">
+        <v>79</v>
+      </c>
+      <c r="E578" t="s">
         <v>4</v>
       </c>
-      <c r="F567" t="s">
-        <v>77</v>
-      </c>
-      <c r="G567" t="s">
+      <c r="F578" t="s">
+        <v>77</v>
+      </c>
+      <c r="G578" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="568" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A568" t="s">
+    <row r="579" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
         <v>100</v>
       </c>
-      <c r="B568">
+      <c r="B579">
         <v>1.6111111111111111E-2</v>
       </c>
-      <c r="C568" t="s">
-        <v>79</v>
-      </c>
-      <c r="E568" t="s">
+      <c r="C579" t="s">
+        <v>79</v>
+      </c>
+      <c r="E579" t="s">
         <v>53</v>
       </c>
-      <c r="F568" t="s">
-        <v>77</v>
-      </c>
-      <c r="G568" t="s">
+      <c r="F579" t="s">
+        <v>77</v>
+      </c>
+      <c r="G579" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="569" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A569" t="s">
+    <row r="580" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
         <v>51</v>
       </c>
-      <c r="B569">
+      <c r="B580">
         <f>1/3.6</f>
         <v>0.27777777777777779</v>
       </c>
-      <c r="C569" t="s">
+      <c r="C580" t="s">
         <v>81</v>
       </c>
-      <c r="E569" t="s">
+      <c r="E580" t="s">
         <v>119</v>
       </c>
-      <c r="F569" t="s">
-        <v>77</v>
-      </c>
-      <c r="G569" t="s">
+      <c r="F580" t="s">
+        <v>77</v>
+      </c>
+      <c r="G580" t="s">
         <v>52</v>
       </c>
-      <c r="H569" t="s">
+      <c r="H580" t="s">
         <v>328</v>
-      </c>
-    </row>
-    <row r="570" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A570" t="s">
-        <v>113</v>
-      </c>
-      <c r="B570">
-        <v>1</v>
-      </c>
-      <c r="C570" t="s">
-        <v>79</v>
-      </c>
-      <c r="E570" t="s">
-        <v>92</v>
-      </c>
-      <c r="F570" t="s">
-        <v>77</v>
-      </c>
-      <c r="G570" t="s">
-        <v>120</v>
-      </c>
-      <c r="H570" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="571" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A571" t="s">
-        <v>389</v>
-      </c>
-      <c r="B571">
-        <v>0.23200000000000001</v>
-      </c>
-      <c r="C571" t="s">
-        <v>135</v>
-      </c>
-      <c r="E571" t="s">
-        <v>92</v>
-      </c>
-      <c r="F571" t="s">
-        <v>77</v>
-      </c>
-      <c r="G571" t="s">
-        <v>390</v>
-      </c>
-      <c r="H571" t="s">
-        <v>388</v>
-      </c>
-    </row>
-    <row r="572" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A572" t="s">
-        <v>114</v>
-      </c>
-      <c r="B572">
-        <v>4</v>
-      </c>
-      <c r="C572" t="s">
-        <v>135</v>
-      </c>
-      <c r="E572" t="s">
-        <v>92</v>
-      </c>
-      <c r="F572" t="s">
-        <v>77</v>
-      </c>
-      <c r="G572" t="s">
-        <v>121</v>
-      </c>
-      <c r="H572" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="573" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A573" t="s">
-        <v>395</v>
-      </c>
-      <c r="B573">
-        <v>0</v>
-      </c>
-      <c r="C573" t="s">
-        <v>79</v>
-      </c>
-      <c r="D573" t="s">
-        <v>62</v>
-      </c>
-      <c r="F573" t="s">
-        <v>78</v>
-      </c>
-      <c r="H573" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="574" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A574" t="s">
-        <v>396</v>
-      </c>
-      <c r="B574">
-        <v>0</v>
-      </c>
-      <c r="C574" t="s">
-        <v>79</v>
-      </c>
-      <c r="D574" t="s">
-        <v>62</v>
-      </c>
-      <c r="F574" t="s">
-        <v>78</v>
-      </c>
-      <c r="H574" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="575" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A575" t="s">
-        <v>397</v>
-      </c>
-      <c r="B575">
-        <v>0</v>
-      </c>
-      <c r="C575" t="s">
-        <v>79</v>
-      </c>
-      <c r="D575" t="s">
-        <v>62</v>
-      </c>
-      <c r="F575" t="s">
-        <v>78</v>
-      </c>
-      <c r="H575" t="s">
-        <v>393</v>
-      </c>
-    </row>
-    <row r="576" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A576" t="s">
-        <v>398</v>
-      </c>
-      <c r="B576">
-        <v>0</v>
-      </c>
-      <c r="C576" t="s">
-        <v>79</v>
-      </c>
-      <c r="D576" t="s">
-        <v>62</v>
-      </c>
-      <c r="F576" t="s">
-        <v>78</v>
-      </c>
-      <c r="H576" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="579" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A579" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B579" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="580" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A580" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B580" s="5" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="581" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>3</v>
-      </c>
-      <c r="B581" t="s">
+        <v>113</v>
+      </c>
+      <c r="B581">
+        <v>1</v>
+      </c>
+      <c r="C581" t="s">
+        <v>79</v>
+      </c>
+      <c r="E581" t="s">
         <v>92</v>
+      </c>
+      <c r="F581" t="s">
+        <v>77</v>
+      </c>
+      <c r="G581" t="s">
+        <v>120</v>
+      </c>
+      <c r="H581" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="582" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A582" t="s">
-        <v>5</v>
+        <v>389</v>
       </c>
       <c r="B582">
-        <v>1</v>
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="C582" t="s">
+        <v>135</v>
+      </c>
+      <c r="E582" t="s">
+        <v>92</v>
+      </c>
+      <c r="F582" t="s">
+        <v>77</v>
+      </c>
+      <c r="G582" t="s">
+        <v>390</v>
+      </c>
+      <c r="H582" t="s">
+        <v>388</v>
       </c>
     </row>
     <row r="583" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A583" t="s">
-        <v>6</v>
-      </c>
-      <c r="B583" t="s">
-        <v>145</v>
+        <v>114</v>
+      </c>
+      <c r="B583">
+        <v>4</v>
+      </c>
+      <c r="C583" t="s">
+        <v>135</v>
+      </c>
+      <c r="E583" t="s">
+        <v>92</v>
+      </c>
+      <c r="F583" t="s">
+        <v>77</v>
+      </c>
+      <c r="G583" t="s">
+        <v>121</v>
+      </c>
+      <c r="H583" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="584" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A584" t="s">
-        <v>7</v>
-      </c>
-      <c r="B584" t="s">
-        <v>7</v>
+        <v>395</v>
+      </c>
+      <c r="B584">
+        <v>0</v>
+      </c>
+      <c r="C584" t="s">
+        <v>79</v>
+      </c>
+      <c r="D584" t="s">
+        <v>62</v>
+      </c>
+      <c r="F584" t="s">
+        <v>78</v>
+      </c>
+      <c r="H584" t="s">
+        <v>391</v>
       </c>
     </row>
     <row r="585" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A585" t="s">
+        <v>396</v>
+      </c>
+      <c r="B585">
+        <v>0</v>
+      </c>
+      <c r="C585" t="s">
+        <v>79</v>
+      </c>
+      <c r="D585" t="s">
+        <v>62</v>
+      </c>
+      <c r="F585" t="s">
+        <v>78</v>
+      </c>
+      <c r="H585" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="586" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A586" t="s">
+        <v>397</v>
+      </c>
+      <c r="B586">
+        <v>0</v>
+      </c>
+      <c r="C586" t="s">
+        <v>79</v>
+      </c>
+      <c r="D586" t="s">
+        <v>62</v>
+      </c>
+      <c r="F586" t="s">
+        <v>78</v>
+      </c>
+      <c r="H586" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="587" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A587" t="s">
+        <v>398</v>
+      </c>
+      <c r="B587">
+        <v>0</v>
+      </c>
+      <c r="C587" t="s">
+        <v>79</v>
+      </c>
+      <c r="D587" t="s">
+        <v>62</v>
+      </c>
+      <c r="F587" t="s">
+        <v>78</v>
+      </c>
+      <c r="H587" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="590" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A590" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B590" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="591" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A591" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B591" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="592" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>3</v>
+      </c>
+      <c r="B592" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="593" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>5</v>
+      </c>
+      <c r="B593">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="594" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>6</v>
+      </c>
+      <c r="B594" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="595" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>7</v>
+      </c>
+      <c r="B595" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="596" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
         <v>8</v>
       </c>
-      <c r="B585" t="s">
+      <c r="B596" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="586" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A586" s="1" t="s">
+    <row r="597" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A597" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B586" s="1"/>
-      <c r="C586" s="1"/>
-      <c r="D586" s="1"/>
-      <c r="E586" s="1"/>
-      <c r="F586" s="1"/>
-      <c r="G586" s="1"/>
-    </row>
-    <row r="587" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A587" s="1" t="s">
+      <c r="B597" s="1"/>
+      <c r="C597" s="1"/>
+      <c r="D597" s="1"/>
+      <c r="E597" s="1"/>
+      <c r="F597" s="1"/>
+      <c r="G597" s="1"/>
+    </row>
+    <row r="598" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A598" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B587" s="1" t="s">
+      <c r="B598" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C587" s="1" t="s">
+      <c r="C598" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D587" s="1" t="s">
+      <c r="D598" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E587" s="1" t="s">
+      <c r="E598" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F587" s="1" t="s">
+      <c r="F598" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G587" s="1" t="s">
+      <c r="G598" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H587" s="1" t="s">
+      <c r="H598" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="588" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A588" t="str">
-        <f>B579</f>
+    <row r="599" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A599" t="str">
+        <f>B590</f>
         <v>tray cleaning, for perovskite</v>
       </c>
-      <c r="B588">
+      <c r="B599">
         <f>34866218.5922179/34866218.5922179</f>
         <v>1</v>
       </c>
-      <c r="C588" t="s">
+      <c r="C599" t="s">
         <v>7</v>
       </c>
-      <c r="E588" t="s">
+      <c r="E599" t="s">
         <v>92</v>
       </c>
-      <c r="F588" t="s">
+      <c r="F599" t="s">
         <v>14</v>
       </c>
-      <c r="G588" t="str">
-        <f>B583</f>
+      <c r="G599" t="str">
+        <f>B594</f>
         <v>tray cleaning</v>
       </c>
-      <c r="H588" t="s">
+      <c r="H599" t="s">
         <v>316</v>
       </c>
     </row>
-    <row r="589" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A589" t="s">
+    <row r="600" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
         <v>364</v>
       </c>
-      <c r="B589">
+      <c r="B600">
         <f>2.10977682373547E-07/0.7</f>
         <v>3.0139668910506718E-7</v>
       </c>
-      <c r="C589" t="s">
-        <v>79</v>
-      </c>
-      <c r="E589" t="s">
+      <c r="C600" t="s">
+        <v>79</v>
+      </c>
+      <c r="E600" t="s">
         <v>53</v>
       </c>
-      <c r="F589" t="s">
-        <v>77</v>
-      </c>
-      <c r="G589" t="s">
+      <c r="F600" t="s">
+        <v>77</v>
+      </c>
+      <c r="G600" t="s">
         <v>365</v>
       </c>
-      <c r="H589" t="s">
+      <c r="H600" t="s">
         <v>363</v>
       </c>
     </row>
-    <row r="590" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A590" t="s">
+    <row r="601" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A601" t="s">
         <v>100</v>
       </c>
-      <c r="B590">
+      <c r="B601">
         <f>0.0000372313557129788</f>
         <v>3.7231355712978797E-5</v>
       </c>
-      <c r="C590" t="s">
-        <v>79</v>
-      </c>
-      <c r="E590" t="s">
+      <c r="C601" t="s">
+        <v>79</v>
+      </c>
+      <c r="E601" t="s">
         <v>53</v>
       </c>
-      <c r="F590" t="s">
-        <v>77</v>
-      </c>
-      <c r="G590" t="s">
+      <c r="F601" t="s">
+        <v>77</v>
+      </c>
+      <c r="G601" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="591" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A591" t="s">
+    <row r="602" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A602" t="s">
         <v>51</v>
       </c>
-      <c r="B591">
+      <c r="B602">
         <f>0.0268065761133448/3.6</f>
         <v>7.446271142595778E-3</v>
       </c>
-      <c r="C591" t="s">
+      <c r="C602" t="s">
         <v>81</v>
       </c>
-      <c r="E591" t="s">
+      <c r="E602" t="s">
         <v>119</v>
       </c>
-      <c r="F591" t="s">
-        <v>77</v>
-      </c>
-      <c r="G591" t="s">
+      <c r="F602" t="s">
+        <v>77</v>
+      </c>
+      <c r="G602" t="s">
         <v>52</v>
       </c>
-      <c r="H591" t="s">
+      <c r="H602" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="592" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A592" t="s">
+    <row r="603" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A603" t="s">
         <v>366</v>
       </c>
-      <c r="B592">
+      <c r="B603">
         <f>3.97134460938441E-06*1000</f>
         <v>3.97134460938441E-3</v>
       </c>
-      <c r="C592" t="s">
-        <v>79</v>
-      </c>
-      <c r="E592" t="s">
+      <c r="C603" t="s">
+        <v>79</v>
+      </c>
+      <c r="E603" t="s">
         <v>119</v>
       </c>
-      <c r="F592" t="s">
-        <v>77</v>
-      </c>
-      <c r="G592" t="s">
+      <c r="F603" t="s">
+        <v>77</v>
+      </c>
+      <c r="G603" t="s">
         <v>59</v>
       </c>
-      <c r="H592" t="s">
+      <c r="H603" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="593" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A593" t="s">
+    <row r="604" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A604" t="s">
         <v>93</v>
       </c>
-      <c r="B593">
+      <c r="B604">
         <f>0.000191120959326625</f>
         <v>1.91120959326625E-4</v>
       </c>
-      <c r="C593" t="s">
+      <c r="C604" t="s">
         <v>96</v>
       </c>
-      <c r="E593" t="s">
+      <c r="E604" t="s">
         <v>4</v>
       </c>
-      <c r="F593" t="s">
-        <v>77</v>
-      </c>
-      <c r="G593" t="s">
+      <c r="F604" t="s">
+        <v>77</v>
+      </c>
+      <c r="G604" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="594" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A594" t="s">
+    <row r="605" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A605" t="s">
         <v>368</v>
       </c>
-      <c r="B594">
+      <c r="B605">
         <f>-2.48209038086526E-06</f>
         <v>-2.48209038086526E-6</v>
       </c>
-      <c r="C594" t="s">
+      <c r="C605" t="s">
         <v>135</v>
       </c>
-      <c r="E594" t="s">
+      <c r="E605" t="s">
         <v>54</v>
       </c>
-      <c r="F594" t="s">
-        <v>77</v>
-      </c>
-      <c r="G594" t="s">
+      <c r="F605" t="s">
+        <v>77</v>
+      </c>
+      <c r="G605" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="595" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A595" s="8" t="s">
+    <row r="606" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A606" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="B595">
+      <c r="B606">
         <f>-0.148925422851915</f>
         <v>-0.14892542285191501</v>
       </c>
-      <c r="C595" t="s">
+      <c r="C606" t="s">
         <v>135</v>
       </c>
-      <c r="E595" t="s">
+      <c r="E606" t="s">
         <v>92</v>
       </c>
-      <c r="F595" t="s">
-        <v>77</v>
-      </c>
-      <c r="G595" t="s">
+      <c r="F606" t="s">
+        <v>77</v>
+      </c>
+      <c r="G606" t="s">
         <v>410</v>
       </c>
-      <c r="H595" t="s">
+      <c r="H606" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="598" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A598" s="2" t="s">
+    <row r="609" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A609" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B598" s="1" t="s">
+      <c r="B609" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="599" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A599" s="5" t="s">
+    <row r="610" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A610" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B599" s="5" t="s">
+      <c r="B610" s="5" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="600" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A600" t="s">
+    <row r="611" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A611" t="s">
         <v>3</v>
       </c>
-      <c r="B600" t="s">
+      <c r="B611" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="601" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A601" t="s">
+    <row r="612" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A612" t="s">
         <v>5</v>
       </c>
-      <c r="B601">
+      <c r="B612">
         <v>1</v>
       </c>
     </row>
-    <row r="602" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A602" t="s">
+    <row r="613" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A613" t="s">
         <v>6</v>
       </c>
-      <c r="B602" t="s">
+      <c r="B613" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="603" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A603" t="s">
+    <row r="614" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A614" t="s">
         <v>7</v>
       </c>
-      <c r="B603" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="604" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A604" t="s">
+      <c r="B614" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="615" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A615" t="s">
         <v>8</v>
       </c>
-      <c r="B604" t="s">
+      <c r="B615" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="605" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A605" s="1" t="s">
+    <row r="616" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A616" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B605" s="1"/>
-      <c r="C605" s="1"/>
-      <c r="D605" s="1"/>
-      <c r="E605" s="1"/>
-      <c r="F605" s="1"/>
-      <c r="G605" s="1"/>
-    </row>
-    <row r="606" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A606" s="1" t="s">
+      <c r="B616" s="1"/>
+      <c r="C616" s="1"/>
+      <c r="D616" s="1"/>
+      <c r="E616" s="1"/>
+      <c r="F616" s="1"/>
+      <c r="G616" s="1"/>
+    </row>
+    <row r="617" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A617" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B606" s="1" t="s">
+      <c r="B617" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C606" s="1" t="s">
+      <c r="C617" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D606" s="1" t="s">
+      <c r="D617" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E606" s="1" t="s">
+      <c r="E617" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F606" s="1" t="s">
+      <c r="F617" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G606" s="1" t="s">
+      <c r="G617" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H606" s="1" t="s">
+      <c r="H617" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="607" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A607" t="str">
-        <f>B598</f>
+    <row r="618" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A618" t="str">
+        <f>B609</f>
         <v>ultrapure water system activity, for perovskite</v>
       </c>
-      <c r="B607">
+      <c r="B618">
         <f>2307.27272727273/2307.27272727273</f>
         <v>1</v>
       </c>
-      <c r="C607" t="s">
-        <v>79</v>
-      </c>
-      <c r="E607" t="s">
+      <c r="C618" t="s">
+        <v>79</v>
+      </c>
+      <c r="E618" t="s">
         <v>92</v>
       </c>
-      <c r="F607" t="s">
+      <c r="F618" t="s">
         <v>14</v>
       </c>
-      <c r="G607" t="str">
-        <f>B602</f>
+      <c r="G618" t="str">
+        <f>B613</f>
         <v>ultra pure water</v>
       </c>
-      <c r="H607" t="s">
+      <c r="H618" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="608" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A608" t="s">
+    <row r="619" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A619" t="s">
         <v>51</v>
       </c>
-      <c r="B608">
+      <c r="B619">
         <f>26.1818181818182/3.6/2307.27272727273</f>
         <v>3.1520882584712352E-3</v>
       </c>
-      <c r="C608" t="s">
+      <c r="C619" t="s">
         <v>81</v>
       </c>
-      <c r="E608" t="s">
+      <c r="E619" t="s">
         <v>119</v>
       </c>
-      <c r="F608" t="s">
-        <v>77</v>
-      </c>
-      <c r="G608" t="s">
+      <c r="F619" t="s">
+        <v>77</v>
+      </c>
+      <c r="G619" t="s">
         <v>52</v>
       </c>
-      <c r="H608" t="s">
+      <c r="H619" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="609" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A609" t="s">
+    <row r="620" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A620" t="s">
         <v>366</v>
       </c>
-      <c r="B609">
+      <c r="B620">
         <f>3.63854545454545*1000/2307.27272727273</f>
         <v>1.576989755713156</v>
       </c>
-      <c r="C609" t="s">
-        <v>79</v>
-      </c>
-      <c r="E609" t="s">
+      <c r="C620" t="s">
+        <v>79</v>
+      </c>
+      <c r="E620" t="s">
         <v>119</v>
       </c>
-      <c r="F609" t="s">
-        <v>77</v>
-      </c>
-      <c r="G609" t="s">
+      <c r="F620" t="s">
+        <v>77</v>
+      </c>
+      <c r="G620" t="s">
         <v>59</v>
       </c>
-      <c r="H609" t="s">
+      <c r="H620" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="610" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A610" t="s">
+    <row r="621" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A621" t="s">
         <v>114</v>
       </c>
-      <c r="B610">
+      <c r="B621">
         <f>0.00109090909090909/2307.27272727273</f>
         <v>4.7281323877068463E-7</v>
       </c>
-      <c r="C610" t="s">
+      <c r="C621" t="s">
         <v>135</v>
       </c>
-      <c r="E610" t="s">
+      <c r="E621" t="s">
         <v>92</v>
       </c>
-      <c r="F610" t="s">
-        <v>77</v>
-      </c>
-      <c r="G610" t="s">
+      <c r="F621" t="s">
+        <v>77</v>
+      </c>
+      <c r="G621" t="s">
         <v>121</v>
       </c>
-      <c r="H610" t="s">
+      <c r="H621" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="611" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A611" t="s">
+    <row r="622" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A622" t="s">
         <v>369</v>
       </c>
-      <c r="B611">
+      <c r="B622">
         <f>3.27272727272727E-07/2307.27272727273</f>
         <v>1.4184397163120539E-10</v>
       </c>
-      <c r="C611" t="s">
+      <c r="C622" t="s">
         <v>7</v>
       </c>
-      <c r="E611" t="s">
+      <c r="E622" t="s">
         <v>54</v>
       </c>
-      <c r="F611" t="s">
-        <v>77</v>
-      </c>
-      <c r="G611" t="s">
+      <c r="F622" t="s">
+        <v>77</v>
+      </c>
+      <c r="G622" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="612" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A612" t="s">
+    <row r="623" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A623" t="s">
         <v>258</v>
       </c>
-      <c r="B612">
+      <c r="B623">
         <f>-1/2307.27272727273</f>
         <v>-4.3341213553979455E-4</v>
       </c>
-      <c r="C612" t="s">
+      <c r="C623" t="s">
         <v>135</v>
       </c>
-      <c r="E612" t="s">
+      <c r="E623" t="s">
         <v>119</v>
       </c>
-      <c r="F612" t="s">
-        <v>77</v>
-      </c>
-      <c r="G612" t="s">
+      <c r="F623" t="s">
+        <v>77</v>
+      </c>
+      <c r="G623" t="s">
         <v>259</v>
       </c>
-      <c r="H612" t="s">
+      <c r="H623" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="615" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A615" s="2" t="s">
+    <row r="626" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A626" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B615" s="1" t="s">
+      <c r="B626" s="1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="616" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A616" s="5" t="s">
+    <row r="627" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A627" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B616" s="5" t="s">
+      <c r="B627" s="5" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="617" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A617" t="s">
+    <row r="628" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A628" t="s">
         <v>3</v>
       </c>
-      <c r="B617" t="s">
+      <c r="B628" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="618" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A618" t="s">
+    <row r="629" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A629" t="s">
         <v>5</v>
       </c>
-      <c r="B618">
+      <c r="B629">
         <v>1</v>
       </c>
     </row>
-    <row r="619" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A619" t="s">
+    <row r="630" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A630" t="s">
         <v>6</v>
       </c>
-      <c r="B619" t="s">
+      <c r="B630" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="620" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A620" t="s">
+    <row r="631" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A631" t="s">
         <v>7</v>
       </c>
-      <c r="B620" t="s">
+      <c r="B631" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="621" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A621" t="s">
+    <row r="632" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A632" t="s">
         <v>8</v>
       </c>
-      <c r="B621" t="s">
+      <c r="B632" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="622" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A622" s="1" t="s">
+    <row r="633" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A633" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B622" s="1"/>
-      <c r="C622" s="1"/>
-      <c r="D622" s="1"/>
-      <c r="E622" s="1"/>
-      <c r="F622" s="1"/>
-      <c r="G622" s="1"/>
-    </row>
-    <row r="623" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A623" s="1" t="s">
+      <c r="B633" s="1"/>
+      <c r="C633" s="1"/>
+      <c r="D633" s="1"/>
+      <c r="E633" s="1"/>
+      <c r="F633" s="1"/>
+      <c r="G633" s="1"/>
+    </row>
+    <row r="634" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A634" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B623" s="1" t="s">
+      <c r="B634" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C623" s="1" t="s">
+      <c r="C634" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D623" s="1" t="s">
+      <c r="D634" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E623" s="1" t="s">
+      <c r="E634" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F623" s="1" t="s">
+      <c r="F634" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G623" s="1" t="s">
+      <c r="G634" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H623" s="1" t="s">
+      <c r="H634" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="624" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A624" t="str">
-        <f>B615</f>
+    <row r="635" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A635" t="str">
+        <f>B626</f>
         <v>inhouse waste water treatment, for perovskite production</v>
       </c>
-      <c r="B624">
+      <c r="B635">
         <f>-1</f>
         <v>-1</v>
       </c>
-      <c r="C624" t="str">
-        <f>B620</f>
+      <c r="C635" t="str">
+        <f>B631</f>
         <v>cubic meter</v>
       </c>
-      <c r="E624" t="s">
+      <c r="E635" t="s">
         <v>92</v>
       </c>
-      <c r="F624" t="s">
+      <c r="F635" t="s">
         <v>14</v>
       </c>
-      <c r="G624" t="str">
-        <f>B619</f>
+      <c r="G635" t="str">
+        <f>B630</f>
         <v>waste water</v>
       </c>
-      <c r="H624" t="s">
+      <c r="H635" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="625" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A625" t="s">
+    <row r="636" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A636" t="s">
         <v>104</v>
       </c>
-      <c r="B625">
+      <c r="B636">
         <f>0.000170225710878426/0.7*1149.2</f>
         <v>0.27946198134498168</v>
       </c>
-      <c r="C625" t="s">
-        <v>79</v>
-      </c>
-      <c r="E625" t="s">
+      <c r="C636" t="s">
+        <v>79</v>
+      </c>
+      <c r="E636" t="s">
         <v>53</v>
       </c>
-      <c r="F625" t="s">
-        <v>77</v>
-      </c>
-      <c r="G625" t="s">
+      <c r="F636" t="s">
+        <v>77</v>
+      </c>
+      <c r="G636" t="s">
         <v>105</v>
       </c>
-      <c r="H625" t="s">
+      <c r="H636" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="626" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A626" t="s">
+    <row r="637" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A637" t="s">
         <v>100</v>
       </c>
-      <c r="B626">
+      <c r="B637">
         <v>0.30262348600609101</v>
       </c>
-      <c r="C626" t="s">
-        <v>79</v>
-      </c>
-      <c r="E626" t="s">
+      <c r="C637" t="s">
+        <v>79</v>
+      </c>
+      <c r="E637" t="s">
         <v>53</v>
       </c>
-      <c r="F626" t="s">
-        <v>77</v>
-      </c>
-      <c r="G626" t="s">
+      <c r="F637" t="s">
+        <v>77</v>
+      </c>
+      <c r="G637" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="627" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A627" t="s">
+    <row r="638" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A638" t="s">
         <v>25</v>
       </c>
-      <c r="B627">
+      <c r="B638">
         <f>0.739952718676123*1.52</f>
         <v>1.124728132387707</v>
       </c>
-      <c r="C627" t="s">
-        <v>79</v>
-      </c>
-      <c r="E627" t="s">
+      <c r="C638" t="s">
+        <v>79</v>
+      </c>
+      <c r="E638" t="s">
         <v>4</v>
       </c>
-      <c r="F627" t="s">
-        <v>77</v>
-      </c>
-      <c r="G627" t="s">
+      <c r="F638" t="s">
+        <v>77</v>
+      </c>
+      <c r="G638" t="s">
         <v>111</v>
       </c>
-      <c r="H627" t="s">
+      <c r="H638" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="628" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A628" t="s">
+    <row r="639" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A639" t="s">
         <v>374</v>
       </c>
-      <c r="B628">
+      <c r="B639">
         <v>0.45705279747832939</v>
       </c>
-      <c r="C628" t="s">
-        <v>79</v>
-      </c>
-      <c r="E628" t="s">
+      <c r="C639" t="s">
+        <v>79</v>
+      </c>
+      <c r="E639" t="s">
         <v>4</v>
       </c>
-      <c r="F628" t="s">
-        <v>77</v>
-      </c>
-      <c r="G628" t="s">
+      <c r="F639" t="s">
+        <v>77</v>
+      </c>
+      <c r="G639" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="629" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A629" t="s">
+    <row r="640" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A640" t="s">
         <v>375</v>
       </c>
-      <c r="B629">
+      <c r="B640">
         <v>0.33884948778565799</v>
       </c>
-      <c r="C629" t="s">
-        <v>79</v>
-      </c>
-      <c r="E629" t="s">
+      <c r="C640" t="s">
+        <v>79</v>
+      </c>
+      <c r="E640" t="s">
         <v>53</v>
       </c>
-      <c r="F629" t="s">
-        <v>77</v>
-      </c>
-      <c r="G629" t="s">
+      <c r="F640" t="s">
+        <v>77</v>
+      </c>
+      <c r="G640" t="s">
         <v>378</v>
       </c>
     </row>
-    <row r="630" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A630" t="s">
+    <row r="641" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A641" t="s">
         <v>376</v>
       </c>
-      <c r="B630">
+      <c r="B641">
         <v>0.42111899133175729</v>
       </c>
-      <c r="C630" t="s">
-        <v>79</v>
-      </c>
-      <c r="E630" t="s">
+      <c r="C641" t="s">
+        <v>79</v>
+      </c>
+      <c r="E641" t="s">
         <v>53</v>
       </c>
-      <c r="F630" t="s">
-        <v>77</v>
-      </c>
-      <c r="G630" t="s">
+      <c r="F641" t="s">
+        <v>77</v>
+      </c>
+      <c r="G641" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="631" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A631" t="s">
+    <row r="642" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A642" t="s">
         <v>51</v>
       </c>
-      <c r="B631">
+      <c r="B642">
         <f>78.8022064617809/3.6</f>
         <v>21.88950179493914</v>
       </c>
-      <c r="C631" t="s">
+      <c r="C642" t="s">
         <v>81</v>
       </c>
-      <c r="E631" t="s">
+      <c r="E642" t="s">
         <v>119</v>
       </c>
-      <c r="F631" t="s">
-        <v>77</v>
-      </c>
-      <c r="G631" t="s">
+      <c r="F642" t="s">
+        <v>77</v>
+      </c>
+      <c r="G642" t="s">
         <v>52</v>
       </c>
-      <c r="H631" t="s">
+      <c r="H642" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="632" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A632" t="s">
+    <row r="643" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A643" t="s">
         <v>114</v>
       </c>
-      <c r="B632">
+      <c r="B643">
         <f>78.8022064617809</f>
         <v>78.802206461780898</v>
       </c>
-      <c r="C632" t="s">
+      <c r="C643" t="s">
         <v>135</v>
       </c>
-      <c r="E632" t="s">
+      <c r="E643" t="s">
         <v>92</v>
       </c>
-      <c r="F632" t="s">
-        <v>77</v>
-      </c>
-      <c r="G632" t="s">
+      <c r="F643" t="s">
+        <v>77</v>
+      </c>
+      <c r="G643" t="s">
         <v>121</v>
       </c>
-      <c r="H632" t="s">
+      <c r="H643" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="633" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A633" t="s">
+    <row r="644" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A644" t="s">
         <v>366</v>
       </c>
-      <c r="B633">
+      <c r="B644">
         <v>315.20882584712399</v>
       </c>
-      <c r="C633" t="s">
-        <v>79</v>
-      </c>
-      <c r="E633" t="s">
+      <c r="C644" t="s">
+        <v>79</v>
+      </c>
+      <c r="E644" t="s">
         <v>119</v>
       </c>
-      <c r="F633" t="s">
-        <v>77</v>
-      </c>
-      <c r="G633" t="s">
+      <c r="F644" t="s">
+        <v>77</v>
+      </c>
+      <c r="G644" t="s">
         <v>59</v>
       </c>
-      <c r="H633" t="s">
+      <c r="H644" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="634" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A634" t="s">
+    <row r="645" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A645" t="s">
         <v>258</v>
       </c>
-      <c r="B634">
+      <c r="B645">
         <v>0.68557919621749397</v>
       </c>
-      <c r="C634" t="s">
+      <c r="C645" t="s">
         <v>135</v>
       </c>
-      <c r="E634" t="s">
+      <c r="E645" t="s">
         <v>119</v>
       </c>
-      <c r="F634" t="s">
-        <v>77</v>
-      </c>
-      <c r="G634" t="s">
+      <c r="F645" t="s">
+        <v>77</v>
+      </c>
+      <c r="G645" t="s">
         <v>259</v>
       </c>
-      <c r="H634" t="s">
+      <c r="H645" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="635" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A635" t="s">
+    <row r="646" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A646" t="s">
         <v>380</v>
       </c>
-      <c r="B635">
+      <c r="B646">
         <f>0.179790569157611*1000</f>
         <v>179.790569157611</v>
       </c>
-      <c r="C635" t="s">
-        <v>79</v>
-      </c>
-      <c r="E635" t="s">
+      <c r="C646" t="s">
+        <v>79</v>
+      </c>
+      <c r="E646" t="s">
         <v>119</v>
       </c>
-      <c r="F635" t="s">
-        <v>77</v>
-      </c>
-      <c r="G635" t="s">
+      <c r="F646" t="s">
+        <v>77</v>
+      </c>
+      <c r="G646" t="s">
         <v>381</v>
       </c>
     </row>
-    <row r="636" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A636" t="s">
+    <row r="647" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A647" t="s">
         <v>409</v>
       </c>
-      <c r="B636">
+      <c r="B647">
         <f>-78.8022064617809</f>
         <v>-78.802206461780898</v>
       </c>
-      <c r="C636" t="s">
+      <c r="C647" t="s">
         <v>135</v>
       </c>
-      <c r="E636" t="s">
+      <c r="E647" t="s">
         <v>92</v>
       </c>
-      <c r="F636" t="s">
-        <v>77</v>
-      </c>
-      <c r="G636" t="s">
+      <c r="F647" t="s">
+        <v>77</v>
+      </c>
+      <c r="G647" t="s">
         <v>410</v>
       </c>
-      <c r="H636" t="s">
+      <c r="H647" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="637" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A637" t="s">
+    <row r="648" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A648" t="s">
         <v>412</v>
       </c>
-      <c r="B637">
+      <c r="B648">
         <v>47.281323877068601</v>
       </c>
-      <c r="C637" t="s">
+      <c r="C648" t="s">
         <v>135</v>
       </c>
-      <c r="E637" t="s">
+      <c r="E648" t="s">
         <v>92</v>
       </c>
-      <c r="F637" t="s">
-        <v>77</v>
-      </c>
-      <c r="G637" t="s">
+      <c r="F648" t="s">
+        <v>77</v>
+      </c>
+      <c r="G648" t="s">
         <v>413</v>
       </c>
-      <c r="H637" t="s">
+      <c r="H648" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="640" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A640" s="2" t="s">
+    <row r="651" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A651" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B640" s="1" t="s">
+      <c r="B651" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="641" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A641" s="5" t="s">
+    <row r="652" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A652" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B641" s="5" t="s">
+      <c r="B652" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="642" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A642" t="s">
+    <row r="653" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A653" t="s">
         <v>3</v>
       </c>
-      <c r="B642" t="s">
+      <c r="B653" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="643" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A643" t="s">
+    <row r="654" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A654" t="s">
         <v>5</v>
       </c>
-      <c r="B643">
+      <c r="B654">
         <v>1</v>
       </c>
     </row>
-    <row r="644" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A644" t="s">
+    <row r="655" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A655" t="s">
         <v>6</v>
       </c>
-      <c r="B644" t="s">
+      <c r="B655" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="645" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A645" t="s">
+    <row r="656" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A656" t="s">
         <v>7</v>
       </c>
-      <c r="B645" t="s">
+      <c r="B656" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="646" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A646" t="s">
+    <row r="657" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A657" t="s">
         <v>8</v>
       </c>
-      <c r="B646" t="s">
+      <c r="B657" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="647" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A647" s="1" t="s">
+    <row r="658" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A658" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B647" s="1"/>
-      <c r="C647" s="1"/>
-      <c r="D647" s="1"/>
-      <c r="E647" s="1"/>
-      <c r="F647" s="1"/>
-      <c r="G647" s="1"/>
-    </row>
-    <row r="648" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A648" s="1" t="s">
+      <c r="B658" s="1"/>
+      <c r="C658" s="1"/>
+      <c r="D658" s="1"/>
+      <c r="E658" s="1"/>
+      <c r="F658" s="1"/>
+      <c r="G658" s="1"/>
+    </row>
+    <row r="659" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A659" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B648" s="1" t="s">
+      <c r="B659" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C648" s="1" t="s">
+      <c r="C659" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D648" s="1" t="s">
+      <c r="D659" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E648" s="1" t="s">
+      <c r="E659" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F648" s="1" t="s">
+      <c r="F659" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G648" s="1" t="s">
+      <c r="G659" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H648" s="1" t="s">
+      <c r="H659" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="649" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A649" t="str">
-        <f>B640</f>
+    <row r="660" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A660" t="str">
+        <f>B651</f>
         <v>process cooling, water, for perovskite</v>
       </c>
-      <c r="B649">
+      <c r="B660">
         <v>1</v>
       </c>
-      <c r="C649" t="str">
-        <f>B645</f>
+      <c r="C660" t="str">
+        <f>B656</f>
         <v>cubic meter</v>
       </c>
-      <c r="E649" t="s">
+      <c r="E660" t="s">
         <v>92</v>
       </c>
-      <c r="F649" t="s">
+      <c r="F660" t="s">
         <v>14</v>
       </c>
-      <c r="G649" t="str">
-        <f>B644</f>
+      <c r="G660" t="str">
+        <f>B655</f>
         <v>cooling water, conditioned</v>
       </c>
-      <c r="H649" t="s">
+      <c r="H660" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="650" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A650" t="s">
+    <row r="661" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A661" t="s">
         <v>258</v>
       </c>
-      <c r="B650">
+      <c r="B661">
         <f>0.75</f>
         <v>0.75</v>
       </c>
-      <c r="C650" t="s">
+      <c r="C661" t="s">
         <v>135</v>
       </c>
-      <c r="E650" t="s">
+      <c r="E661" t="s">
         <v>119</v>
       </c>
-      <c r="F650" t="s">
-        <v>77</v>
-      </c>
-      <c r="G650" t="s">
+      <c r="F661" t="s">
+        <v>77</v>
+      </c>
+      <c r="G661" t="s">
         <v>259</v>
       </c>
-      <c r="H650" t="s">
+      <c r="H661" t="s">
         <v>371</v>
       </c>
     </row>
-    <row r="651" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A651" t="s">
+    <row r="662" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A662" t="s">
         <v>51</v>
       </c>
-      <c r="B651">
+      <c r="B662">
         <f>0.165704904993084/3.6</f>
         <v>4.602914027585666E-2</v>
       </c>
-      <c r="C651" t="s">
+      <c r="C662" t="s">
         <v>81</v>
       </c>
-      <c r="E651" t="s">
+      <c r="E662" t="s">
         <v>119</v>
       </c>
-      <c r="F651" t="s">
-        <v>77</v>
-      </c>
-      <c r="G651" t="s">
+      <c r="F662" t="s">
+        <v>77</v>
+      </c>
+      <c r="G662" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="652" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A652" t="s">
+    <row r="663" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A663" t="s">
         <v>366</v>
       </c>
-      <c r="B652">
+      <c r="B663">
         <f>0.252525252525253*1000</f>
         <v>252.52525252525299</v>
       </c>
-      <c r="C652" t="s">
-        <v>79</v>
-      </c>
-      <c r="E652" t="s">
+      <c r="C663" t="s">
+        <v>79</v>
+      </c>
+      <c r="E663" t="s">
         <v>119</v>
       </c>
-      <c r="F652" t="s">
-        <v>77</v>
-      </c>
-      <c r="G652" t="s">
+      <c r="F663" t="s">
+        <v>77</v>
+      </c>
+      <c r="G663" t="s">
         <v>59</v>
       </c>
-      <c r="H652" t="s">
+      <c r="H663" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="654" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A654" s="2" t="s">
+    <row r="665" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A665" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B654" s="1" t="s">
+      <c r="B665" s="1" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="655" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A655" s="5" t="s">
+    <row r="666" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A666" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B655" s="5" t="s">
+      <c r="B666" s="5" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="656" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A656" t="s">
+    <row r="667" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A667" t="s">
         <v>3</v>
       </c>
-      <c r="B656" t="s">
+      <c r="B667" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="657" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A657" t="s">
+    <row r="668" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A668" t="s">
         <v>5</v>
       </c>
-      <c r="B657">
+      <c r="B668">
         <v>1</v>
       </c>
     </row>
-    <row r="658" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A658" t="s">
+    <row r="669" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A669" t="s">
         <v>6</v>
       </c>
-      <c r="B658" t="s">
+      <c r="B669" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="659" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A659" t="s">
+    <row r="670" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A670" t="s">
         <v>7</v>
       </c>
-      <c r="B659" t="s">
+      <c r="B670" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="660" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A660" t="s">
+    <row r="671" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A671" t="s">
         <v>8</v>
       </c>
-      <c r="B660" t="s">
+      <c r="B671" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="661" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A661" s="1" t="s">
+    <row r="672" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A672" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B661" s="1"/>
-      <c r="C661" s="1"/>
-      <c r="D661" s="1"/>
-      <c r="E661" s="1"/>
-      <c r="F661" s="1"/>
-      <c r="G661" s="1"/>
-    </row>
-    <row r="662" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A662" s="1" t="s">
+      <c r="B672" s="1"/>
+      <c r="C672" s="1"/>
+      <c r="D672" s="1"/>
+      <c r="E672" s="1"/>
+      <c r="F672" s="1"/>
+      <c r="G672" s="1"/>
+    </row>
+    <row r="673" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A673" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B662" s="1" t="s">
+      <c r="B673" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C662" s="1" t="s">
+      <c r="C673" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D662" s="1" t="s">
+      <c r="D673" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E662" s="1" t="s">
+      <c r="E673" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F662" s="1" t="s">
+      <c r="F673" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G662" s="1" t="s">
+      <c r="G673" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H662" s="1" t="s">
+      <c r="H673" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="663" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A663" t="str">
-        <f>B654</f>
+    <row r="674" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A674" t="str">
+        <f>B665</f>
         <v>process cooling, water, for perovskite</v>
       </c>
-      <c r="B663">
+      <c r="B674">
         <f>-1</f>
         <v>-1</v>
       </c>
-      <c r="C663" t="str">
-        <f>B659</f>
+      <c r="C674" t="str">
+        <f>B670</f>
         <v>cubic meter</v>
       </c>
-      <c r="E663" t="s">
+      <c r="E674" t="s">
         <v>92</v>
       </c>
-      <c r="F663" t="s">
+      <c r="F674" t="s">
         <v>14</v>
       </c>
-      <c r="G663" t="str">
-        <f>B658</f>
+      <c r="G674" t="str">
+        <f>B669</f>
         <v>cooling water, used</v>
       </c>
-      <c r="H663" t="s">
+      <c r="H674" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="666" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A666" s="2" t="s">
+    <row r="677" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A677" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B666" s="1" t="s">
+      <c r="B677" s="1" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="667" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A667" s="5" t="s">
+    <row r="678" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A678" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B667" s="5" t="s">
+      <c r="B678" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="668" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A668" t="s">
+    <row r="679" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A679" t="s">
         <v>3</v>
       </c>
-      <c r="B668" t="s">
+      <c r="B679" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="669" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A669" t="s">
+    <row r="680" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A680" t="s">
         <v>5</v>
       </c>
-      <c r="B669">
+      <c r="B680">
         <v>1</v>
-      </c>
-    </row>
-    <row r="670" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A670" t="s">
-        <v>6</v>
-      </c>
-      <c r="B670" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="671" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A671" t="s">
-        <v>7</v>
-      </c>
-      <c r="B671" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="672" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A672" t="s">
-        <v>8</v>
-      </c>
-      <c r="B672" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="673" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A673" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B673" s="1"/>
-      <c r="C673" s="1"/>
-      <c r="D673" s="1"/>
-      <c r="E673" s="1"/>
-      <c r="F673" s="1"/>
-      <c r="G673" s="1"/>
-    </row>
-    <row r="674" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A674" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B674" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C674" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D674" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E674" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F674" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G674" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H674" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="675" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A675" t="str">
-        <f>B666</f>
-        <v>air compressor activity, for perovskite</v>
-      </c>
-      <c r="B675">
-        <v>1</v>
-      </c>
-      <c r="C675" t="str">
-        <f>B671</f>
-        <v>cubic meter</v>
-      </c>
-      <c r="E675" t="s">
-        <v>92</v>
-      </c>
-      <c r="F675" t="s">
-        <v>14</v>
-      </c>
-      <c r="G675" t="str">
-        <f>B670</f>
-        <v>compressed air, 14 bar, low efficiency</v>
-      </c>
-      <c r="H675" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="676" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A676" t="s">
-        <v>382</v>
-      </c>
-      <c r="B676">
-        <v>1</v>
-      </c>
-      <c r="C676" t="s">
-        <v>135</v>
-      </c>
-      <c r="E676" t="s">
-        <v>53</v>
-      </c>
-      <c r="F676" t="s">
-        <v>77</v>
-      </c>
-      <c r="G676" t="s">
-        <v>383</v>
-      </c>
-      <c r="H676" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="679" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A679" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B679" s="1" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="680" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A680" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B680" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="681" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A681" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B681" t="s">
-        <v>92</v>
+        <v>121</v>
       </c>
     </row>
     <row r="682" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A682" t="s">
-        <v>5</v>
-      </c>
-      <c r="B682">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="B682" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="683" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A683" t="s">
+        <v>8</v>
+      </c>
+      <c r="B683" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="684" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A684" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B684" s="1"/>
+      <c r="C684" s="1"/>
+      <c r="D684" s="1"/>
+      <c r="E684" s="1"/>
+      <c r="F684" s="1"/>
+      <c r="G684" s="1"/>
+    </row>
+    <row r="685" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A685" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B685" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C685" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D685" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E685" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F685" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G685" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B683" t="s">
+      <c r="H685" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="686" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A686" t="str">
+        <f>B677</f>
+        <v>air compressor activity, for perovskite</v>
+      </c>
+      <c r="B686">
+        <v>1</v>
+      </c>
+      <c r="C686" t="str">
+        <f>B682</f>
+        <v>cubic meter</v>
+      </c>
+      <c r="E686" t="s">
+        <v>92</v>
+      </c>
+      <c r="F686" t="s">
+        <v>14</v>
+      </c>
+      <c r="G686" t="str">
+        <f>B681</f>
+        <v>compressed air, 14 bar, low efficiency</v>
+      </c>
+      <c r="H686" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="687" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A687" t="s">
+        <v>382</v>
+      </c>
+      <c r="B687">
+        <v>1</v>
+      </c>
+      <c r="C687" t="s">
+        <v>135</v>
+      </c>
+      <c r="E687" t="s">
+        <v>53</v>
+      </c>
+      <c r="F687" t="s">
+        <v>77</v>
+      </c>
+      <c r="G687" t="s">
+        <v>383</v>
+      </c>
+      <c r="H687" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="690" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A690" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B690" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="691" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A691" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B691" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="692" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A692" t="s">
+        <v>3</v>
+      </c>
+      <c r="B692" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="693" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A693" t="s">
+        <v>5</v>
+      </c>
+      <c r="B693">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="694" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A694" t="s">
+        <v>6</v>
+      </c>
+      <c r="B694" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="684" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A684" t="s">
+    <row r="695" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A695" t="s">
         <v>7</v>
       </c>
-      <c r="B684" t="s">
+      <c r="B695" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="685" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A685" t="s">
+    <row r="696" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A696" t="s">
         <v>8</v>
       </c>
-      <c r="B685" t="s">
+      <c r="B696" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="686" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A686" s="1" t="s">
+    <row r="697" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A697" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B686" s="1"/>
-      <c r="C686" s="1"/>
-      <c r="D686" s="1"/>
-      <c r="E686" s="1"/>
-      <c r="F686" s="1"/>
-      <c r="G686" s="1"/>
-    </row>
-    <row r="687" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A687" s="1" t="s">
+      <c r="B697" s="1"/>
+      <c r="C697" s="1"/>
+      <c r="D697" s="1"/>
+      <c r="E697" s="1"/>
+      <c r="F697" s="1"/>
+      <c r="G697" s="1"/>
+    </row>
+    <row r="698" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A698" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B687" s="1" t="s">
+      <c r="B698" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C687" s="1" t="s">
+      <c r="C698" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D687" s="1" t="s">
+      <c r="D698" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E687" s="1" t="s">
+      <c r="E698" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F687" s="1" t="s">
+      <c r="F698" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G687" s="1" t="s">
+      <c r="G698" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H687" s="1" t="s">
+      <c r="H698" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="688" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A688" t="str">
-        <f>B679</f>
+    <row r="699" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A699" t="str">
+        <f>B690</f>
         <v>process exhaust ventilators, general, for perovskite production</v>
       </c>
-      <c r="B688">
+      <c r="B699">
         <v>-1</v>
       </c>
-      <c r="C688" t="str">
-        <f>B684</f>
+      <c r="C699" t="str">
+        <f>B695</f>
         <v>cubic meter</v>
       </c>
-      <c r="E688" t="s">
+      <c r="E699" t="s">
         <v>92</v>
       </c>
-      <c r="F688" t="s">
+      <c r="F699" t="s">
         <v>14</v>
       </c>
-      <c r="G688" t="str">
-        <f>B683</f>
+      <c r="G699" t="str">
+        <f>B694</f>
         <v>exhaust, general</v>
       </c>
-      <c r="H688" t="s">
+      <c r="H699" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="689" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A689" t="s">
+    <row r="700" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A700" t="s">
         <v>401</v>
       </c>
-      <c r="B689">
+      <c r="B700">
         <v>7.6051410753669521E-7</v>
       </c>
-      <c r="C689" t="s">
+      <c r="C700" t="s">
         <v>7</v>
       </c>
-      <c r="E689" t="s">
+      <c r="E700" t="s">
         <v>4</v>
       </c>
-      <c r="F689" t="s">
-        <v>77</v>
-      </c>
-      <c r="G689" t="s">
+      <c r="F700" t="s">
+        <v>77</v>
+      </c>
+      <c r="G700" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="690" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A690" t="s">
+    <row r="701" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A701" t="s">
         <v>402</v>
       </c>
-      <c r="B690">
+      <c r="B701">
         <v>7.6051410753669521E-7</v>
       </c>
-      <c r="C690" t="s">
+      <c r="C701" t="s">
         <v>7</v>
       </c>
-      <c r="E690" t="s">
+      <c r="E701" t="s">
         <v>57</v>
       </c>
-      <c r="F690" t="s">
-        <v>77</v>
-      </c>
-      <c r="G690" t="s">
+      <c r="F701" t="s">
+        <v>77</v>
+      </c>
+      <c r="G701" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="691" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A691" t="s">
+    <row r="702" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A702" t="s">
         <v>51</v>
       </c>
-      <c r="B691">
+      <c r="B702">
         <f>0.0061881332397246/3.6</f>
         <v>1.7189258999234999E-3</v>
       </c>
-      <c r="C691" t="s">
+      <c r="C702" t="s">
         <v>81</v>
       </c>
-      <c r="E691" t="s">
+      <c r="E702" t="s">
         <v>119</v>
       </c>
-      <c r="F691" t="s">
-        <v>77</v>
-      </c>
-      <c r="G691" t="s">
+      <c r="F702" t="s">
+        <v>77</v>
+      </c>
+      <c r="G702" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="692" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A692" t="s">
-        <v>408</v>
-      </c>
-      <c r="B692">
-        <v>1.1407711613050422E-5</v>
-      </c>
-      <c r="C692" t="s">
-        <v>79</v>
-      </c>
-      <c r="D692" t="s">
-        <v>62</v>
-      </c>
-      <c r="F692" t="s">
-        <v>78</v>
-      </c>
-      <c r="H692" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="693" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A693" t="s">
-        <v>194</v>
-      </c>
-      <c r="B693">
-        <v>9.8572073921971304E-3</v>
-      </c>
-      <c r="C693" t="s">
-        <v>80</v>
-      </c>
-      <c r="D693" t="s">
-        <v>62</v>
-      </c>
-      <c r="F693" t="s">
-        <v>78</v>
-      </c>
-      <c r="H693" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="694" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A694" t="s">
-        <v>76</v>
-      </c>
-      <c r="B694">
-        <v>3.9926990645676497E-5</v>
-      </c>
-      <c r="C694" t="s">
-        <v>135</v>
-      </c>
-      <c r="D694" t="s">
-        <v>62</v>
-      </c>
-      <c r="F694" t="s">
-        <v>78</v>
-      </c>
-      <c r="H694" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="697" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A697" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B697" s="1" t="s">
-        <v>409</v>
-      </c>
-    </row>
-    <row r="698" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A698" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B698" s="5" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="699" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A699" t="s">
-        <v>3</v>
-      </c>
-      <c r="B699" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="700" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A700" t="s">
-        <v>5</v>
-      </c>
-      <c r="B700">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="701" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A701" t="s">
-        <v>6</v>
-      </c>
-      <c r="B701" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="702" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A702" t="s">
-        <v>7</v>
-      </c>
-      <c r="B702" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="703" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A703" t="s">
+        <v>408</v>
+      </c>
+      <c r="B703">
+        <v>1.1407711613050422E-5</v>
+      </c>
+      <c r="C703" t="s">
+        <v>79</v>
+      </c>
+      <c r="D703" t="s">
+        <v>62</v>
+      </c>
+      <c r="F703" t="s">
+        <v>78</v>
+      </c>
+      <c r="H703" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="704" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A704" t="s">
+        <v>194</v>
+      </c>
+      <c r="B704">
+        <v>9.8572073921971304E-3</v>
+      </c>
+      <c r="C704" t="s">
+        <v>80</v>
+      </c>
+      <c r="D704" t="s">
+        <v>62</v>
+      </c>
+      <c r="F704" t="s">
+        <v>78</v>
+      </c>
+      <c r="H704" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="705" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A705" t="s">
+        <v>76</v>
+      </c>
+      <c r="B705">
+        <v>3.9926990645676497E-5</v>
+      </c>
+      <c r="C705" t="s">
+        <v>135</v>
+      </c>
+      <c r="D705" t="s">
+        <v>62</v>
+      </c>
+      <c r="F705" t="s">
+        <v>78</v>
+      </c>
+      <c r="H705" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="708" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A708" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B708" s="1" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="709" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A709" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B709" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="710" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A710" t="s">
+        <v>3</v>
+      </c>
+      <c r="B710" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="711" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A711" t="s">
+        <v>5</v>
+      </c>
+      <c r="B711">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="712" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A712" t="s">
+        <v>6</v>
+      </c>
+      <c r="B712" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="713" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A713" t="s">
+        <v>7</v>
+      </c>
+      <c r="B713" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="714" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A714" t="s">
         <v>8</v>
       </c>
-      <c r="B703" t="s">
+      <c r="B714" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="704" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A704" s="1" t="s">
+    <row r="715" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A715" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B704" s="1"/>
-      <c r="C704" s="1"/>
-      <c r="D704" s="1"/>
-      <c r="E704" s="1"/>
-      <c r="F704" s="1"/>
-      <c r="G704" s="1"/>
-    </row>
-    <row r="705" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A705" s="1" t="s">
+      <c r="B715" s="1"/>
+      <c r="C715" s="1"/>
+      <c r="D715" s="1"/>
+      <c r="E715" s="1"/>
+      <c r="F715" s="1"/>
+      <c r="G715" s="1"/>
+    </row>
+    <row r="716" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A716" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B705" s="1" t="s">
+      <c r="B716" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C705" s="1" t="s">
+      <c r="C716" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D705" s="1" t="s">
+      <c r="D716" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E705" s="1" t="s">
+      <c r="E716" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F705" s="1" t="s">
+      <c r="F716" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G705" s="1" t="s">
+      <c r="G716" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H705" s="1" t="s">
+      <c r="H716" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="706" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A706" t="str">
-        <f>B697</f>
+    <row r="717" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A717" t="str">
+        <f>B708</f>
         <v>process exhaust ventilators, acidic, for perovskite production</v>
       </c>
-      <c r="B706">
+      <c r="B717">
         <v>-1</v>
       </c>
-      <c r="C706" t="str">
-        <f>B702</f>
+      <c r="C717" t="str">
+        <f>B713</f>
         <v>cubic meter</v>
       </c>
-      <c r="E706" t="s">
+      <c r="E717" t="s">
         <v>92</v>
       </c>
-      <c r="F706" t="s">
+      <c r="F717" t="s">
         <v>14</v>
       </c>
-      <c r="G706" t="str">
-        <f>B701</f>
+      <c r="G717" t="str">
+        <f>B712</f>
         <v>exhaust, acidic</v>
       </c>
-      <c r="H706" t="s">
+      <c r="H717" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="707" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A707" t="s">
+    <row r="718" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A718" t="s">
         <v>401</v>
       </c>
-      <c r="B707">
+      <c r="B718">
         <v>7.6051410753669521E-7</v>
       </c>
-      <c r="C707" t="s">
+      <c r="C718" t="s">
         <v>7</v>
       </c>
-      <c r="E707" t="s">
+      <c r="E718" t="s">
         <v>4</v>
       </c>
-      <c r="F707" t="s">
-        <v>77</v>
-      </c>
-      <c r="G707" t="s">
+      <c r="F718" t="s">
+        <v>77</v>
+      </c>
+      <c r="G718" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="708" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A708" t="s">
+    <row r="719" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A719" t="s">
         <v>402</v>
       </c>
-      <c r="B708">
+      <c r="B719">
         <v>7.6051410753669521E-7</v>
       </c>
-      <c r="C708" t="s">
+      <c r="C719" t="s">
         <v>7</v>
       </c>
-      <c r="E708" t="s">
+      <c r="E719" t="s">
         <v>57</v>
       </c>
-      <c r="F708" t="s">
-        <v>77</v>
-      </c>
-      <c r="G708" t="s">
+      <c r="F719" t="s">
+        <v>77</v>
+      </c>
+      <c r="G719" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="709" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A709" t="s">
+    <row r="720" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A720" t="s">
         <v>51</v>
       </c>
-      <c r="B709">
+      <c r="B720">
         <f>0.0061881332397246/3.6</f>
         <v>1.7189258999234999E-3</v>
       </c>
-      <c r="C709" t="s">
+      <c r="C720" t="s">
         <v>81</v>
       </c>
-      <c r="E709" t="s">
+      <c r="E720" t="s">
         <v>119</v>
       </c>
-      <c r="F709" t="s">
-        <v>77</v>
-      </c>
-      <c r="G709" t="s">
+      <c r="F720" t="s">
+        <v>77</v>
+      </c>
+      <c r="G720" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="710" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A710" t="s">
+    <row r="721" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A721" t="s">
         <v>408</v>
       </c>
-      <c r="B710">
+      <c r="B721">
         <v>1.1407711613050422E-5</v>
       </c>
-      <c r="C710" t="s">
-        <v>79</v>
-      </c>
-      <c r="D710" t="s">
+      <c r="C721" t="s">
+        <v>79</v>
+      </c>
+      <c r="D721" t="s">
         <v>62</v>
       </c>
-      <c r="F710" t="s">
+      <c r="F721" t="s">
         <v>78</v>
       </c>
-      <c r="H710" t="s">
+      <c r="H721" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="711" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A711" t="s">
+    <row r="722" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A722" t="s">
         <v>194</v>
       </c>
-      <c r="B711">
+      <c r="B722">
         <v>9.8572073921971304E-3</v>
       </c>
-      <c r="C711" t="s">
+      <c r="C722" t="s">
         <v>80</v>
       </c>
-      <c r="D711" t="s">
+      <c r="D722" t="s">
         <v>62</v>
       </c>
-      <c r="F711" t="s">
+      <c r="F722" t="s">
         <v>78</v>
       </c>
-      <c r="H711" t="s">
+      <c r="H722" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="712" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A712" t="s">
+    <row r="723" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A723" t="s">
         <v>76</v>
       </c>
-      <c r="B712">
+      <c r="B723">
         <v>3.9926990645676497E-5</v>
       </c>
-      <c r="C712" t="s">
+      <c r="C723" t="s">
         <v>135</v>
       </c>
-      <c r="D712" t="s">
+      <c r="D723" t="s">
         <v>62</v>
       </c>
-      <c r="F712" t="s">
+      <c r="F723" t="s">
         <v>78</v>
       </c>
-      <c r="H712" t="s">
+      <c r="H723" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="713" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A713" t="s">
+    <row r="724" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A724" t="s">
         <v>25</v>
       </c>
-      <c r="B713">
+      <c r="B724">
         <f>0.000382716049382716/0.2*2.13</f>
         <v>4.0759259259259247E-3</v>
       </c>
-      <c r="C713" t="s">
-        <v>79</v>
-      </c>
-      <c r="E713" t="s">
+      <c r="C724" t="s">
+        <v>79</v>
+      </c>
+      <c r="E724" t="s">
         <v>4</v>
       </c>
-      <c r="F713" t="s">
-        <v>77</v>
-      </c>
-      <c r="G713" t="s">
+      <c r="F724" t="s">
+        <v>77</v>
+      </c>
+      <c r="G724" t="s">
         <v>111</v>
       </c>
-      <c r="H713" t="s">
+      <c r="H724" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="714" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A714" t="s">
+    <row r="725" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A725" t="s">
         <v>51</v>
       </c>
-      <c r="B714">
+      <c r="B725">
         <f>0.00911111111111111/3.6</f>
         <v>2.5308641975308639E-3</v>
       </c>
-      <c r="C714" t="s">
+      <c r="C725" t="s">
         <v>81</v>
       </c>
-      <c r="E714" t="s">
+      <c r="E725" t="s">
         <v>119</v>
       </c>
-      <c r="F714" t="s">
-        <v>77</v>
-      </c>
-      <c r="G714" t="s">
+      <c r="F725" t="s">
+        <v>77</v>
+      </c>
+      <c r="G725" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="715" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A715" t="s">
+    <row r="726" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A726" t="s">
         <v>100</v>
       </c>
-      <c r="B715">
+      <c r="B726">
         <v>0.15308641975308601</v>
       </c>
-      <c r="C715" t="s">
-        <v>79</v>
-      </c>
-      <c r="E715" t="s">
+      <c r="C726" t="s">
+        <v>79</v>
+      </c>
+      <c r="E726" t="s">
         <v>53</v>
       </c>
-      <c r="F715" t="s">
-        <v>77</v>
-      </c>
-      <c r="G715" t="s">
+      <c r="F726" t="s">
+        <v>77</v>
+      </c>
+      <c r="G726" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="718" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A718" s="2" t="s">
+    <row r="729" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A729" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B718" s="1" t="s">
+      <c r="B729" s="1" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="719" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A719" s="5" t="s">
+    <row r="730" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A730" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B719" s="5" t="s">
+      <c r="B730" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="720" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A720" t="s">
+    <row r="731" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A731" t="s">
         <v>3</v>
       </c>
-      <c r="B720" t="s">
+      <c r="B731" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="721" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A721" t="s">
+    <row r="732" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A732" t="s">
         <v>5</v>
       </c>
-      <c r="B721">
+      <c r="B732">
         <v>1</v>
       </c>
     </row>
-    <row r="722" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A722" t="s">
+    <row r="733" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A733" t="s">
         <v>6</v>
       </c>
-      <c r="B722" t="s">
+      <c r="B733" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="723" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A723" t="s">
+    <row r="734" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A734" t="s">
         <v>7</v>
       </c>
-      <c r="B723" t="s">
+      <c r="B734" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="724" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A724" t="s">
+    <row r="735" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A735" t="s">
         <v>8</v>
       </c>
-      <c r="B724" t="s">
+      <c r="B735" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="725" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A725" s="1" t="s">
+    <row r="736" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A736" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B725" s="1"/>
-      <c r="C725" s="1"/>
-      <c r="D725" s="1"/>
-      <c r="E725" s="1"/>
-      <c r="F725" s="1"/>
-      <c r="G725" s="1"/>
-    </row>
-    <row r="726" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A726" s="1" t="s">
+      <c r="B736" s="1"/>
+      <c r="C736" s="1"/>
+      <c r="D736" s="1"/>
+      <c r="E736" s="1"/>
+      <c r="F736" s="1"/>
+      <c r="G736" s="1"/>
+    </row>
+    <row r="737" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A737" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B726" s="1" t="s">
+      <c r="B737" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C726" s="1" t="s">
+      <c r="C737" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D726" s="1" t="s">
+      <c r="D737" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E726" s="1" t="s">
+      <c r="E737" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F726" s="1" t="s">
+      <c r="F737" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G726" s="1" t="s">
+      <c r="G737" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H726" s="1" t="s">
+      <c r="H737" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="727" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A727" t="str">
-        <f>B718</f>
+    <row r="738" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A738" t="str">
+        <f>B729</f>
         <v>process exhaust ventilators, caustic, for perovskite production</v>
       </c>
-      <c r="B727">
+      <c r="B738">
         <v>-1</v>
       </c>
-      <c r="C727" t="str">
-        <f>B723</f>
+      <c r="C738" t="str">
+        <f>B734</f>
         <v>cubic meter</v>
       </c>
-      <c r="E727" t="s">
+      <c r="E738" t="s">
         <v>92</v>
       </c>
-      <c r="F727" t="s">
+      <c r="F738" t="s">
         <v>14</v>
       </c>
-      <c r="G727" t="str">
-        <f>B722</f>
+      <c r="G738" t="str">
+        <f>B733</f>
         <v>exhaust, caustic</v>
       </c>
-      <c r="H727" t="s">
+      <c r="H738" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="728" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A728" t="s">
+    <row r="739" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
         <v>401</v>
       </c>
-      <c r="B728">
+      <c r="B739">
         <v>7.6051410753669521E-7</v>
       </c>
-      <c r="C728" t="s">
+      <c r="C739" t="s">
         <v>7</v>
       </c>
-      <c r="E728" t="s">
+      <c r="E739" t="s">
         <v>4</v>
       </c>
-      <c r="F728" t="s">
-        <v>77</v>
-      </c>
-      <c r="G728" t="s">
+      <c r="F739" t="s">
+        <v>77</v>
+      </c>
+      <c r="G739" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="729" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A729" t="s">
+    <row r="740" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
         <v>402</v>
       </c>
-      <c r="B729">
+      <c r="B740">
         <v>7.6051410753669521E-7</v>
       </c>
-      <c r="C729" t="s">
+      <c r="C740" t="s">
         <v>7</v>
       </c>
-      <c r="E729" t="s">
+      <c r="E740" t="s">
         <v>57</v>
       </c>
-      <c r="F729" t="s">
-        <v>77</v>
-      </c>
-      <c r="G729" t="s">
+      <c r="F740" t="s">
+        <v>77</v>
+      </c>
+      <c r="G740" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="730" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A730" t="s">
+    <row r="741" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
         <v>51</v>
       </c>
-      <c r="B730">
+      <c r="B741">
         <f>0.0061881332397246/3.6</f>
         <v>1.7189258999234999E-3</v>
       </c>
-      <c r="C730" t="s">
+      <c r="C741" t="s">
         <v>81</v>
       </c>
-      <c r="E730" t="s">
+      <c r="E741" t="s">
         <v>119</v>
       </c>
-      <c r="F730" t="s">
-        <v>77</v>
-      </c>
-      <c r="G730" t="s">
+      <c r="F741" t="s">
+        <v>77</v>
+      </c>
+      <c r="G741" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="731" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A731" t="s">
+    <row r="742" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A742" t="s">
         <v>408</v>
       </c>
-      <c r="B731">
+      <c r="B742">
         <v>1.1407711613050422E-5</v>
       </c>
-      <c r="C731" t="s">
-        <v>79</v>
-      </c>
-      <c r="D731" t="s">
+      <c r="C742" t="s">
+        <v>79</v>
+      </c>
+      <c r="D742" t="s">
         <v>62</v>
       </c>
-      <c r="F731" t="s">
+      <c r="F742" t="s">
         <v>78</v>
       </c>
-      <c r="H731" t="s">
+      <c r="H742" t="s">
         <v>405</v>
       </c>
     </row>
-    <row r="732" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A732" t="s">
+    <row r="743" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
         <v>194</v>
       </c>
-      <c r="B732">
+      <c r="B743">
         <v>9.8572073921971304E-3</v>
       </c>
-      <c r="C732" t="s">
+      <c r="C743" t="s">
         <v>80</v>
       </c>
-      <c r="D732" t="s">
+      <c r="D743" t="s">
         <v>62</v>
       </c>
-      <c r="F732" t="s">
+      <c r="F743" t="s">
         <v>78</v>
       </c>
-      <c r="H732" t="s">
+      <c r="H743" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="733" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A733" t="s">
+    <row r="744" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A744" t="s">
         <v>76</v>
       </c>
-      <c r="B733">
+      <c r="B744">
         <v>3.9926990645676497E-5</v>
       </c>
-      <c r="C733" t="s">
+      <c r="C744" t="s">
         <v>135</v>
       </c>
-      <c r="D733" t="s">
+      <c r="D744" t="s">
         <v>62</v>
       </c>
-      <c r="F733" t="s">
+      <c r="F744" t="s">
         <v>78</v>
       </c>
-      <c r="H733" t="s">
+      <c r="H744" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="734" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A734" t="s">
+    <row r="745" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
         <v>235</v>
       </c>
-      <c r="B734">
+      <c r="B745">
         <f>0.000382716049382716/0.2*1.83</f>
         <v>3.5018518518518515E-3</v>
       </c>
-      <c r="C734" t="s">
-        <v>79</v>
-      </c>
-      <c r="E734" t="s">
+      <c r="C745" t="s">
+        <v>79</v>
+      </c>
+      <c r="E745" t="s">
         <v>53</v>
       </c>
-      <c r="F734" t="s">
-        <v>77</v>
-      </c>
-      <c r="G734" t="s">
+      <c r="F745" t="s">
+        <v>77</v>
+      </c>
+      <c r="G745" t="s">
         <v>414</v>
       </c>
-      <c r="H734" t="s">
+      <c r="H745" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="735" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A735" t="s">
+    <row r="746" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
         <v>51</v>
       </c>
-      <c r="B735">
+      <c r="B746">
         <f>0.0113684210526316/3.6</f>
         <v>3.1578947368421113E-3</v>
       </c>
-      <c r="C735" t="s">
+      <c r="C746" t="s">
         <v>81</v>
       </c>
-      <c r="E735" t="s">
+      <c r="E746" t="s">
         <v>119</v>
       </c>
-      <c r="F735" t="s">
-        <v>77</v>
-      </c>
-      <c r="G735" t="s">
+      <c r="F746" t="s">
+        <v>77</v>
+      </c>
+      <c r="G746" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="736" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A736" t="s">
+    <row r="747" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A747" t="s">
         <v>100</v>
       </c>
-      <c r="B736">
+      <c r="B747">
         <v>0.11184210526315801</v>
       </c>
-      <c r="C736" t="s">
-        <v>79</v>
-      </c>
-      <c r="E736" t="s">
+      <c r="C747" t="s">
+        <v>79</v>
+      </c>
+      <c r="E747" t="s">
         <v>53</v>
       </c>
-      <c r="F736" t="s">
-        <v>77</v>
-      </c>
-      <c r="G736" t="s">
+      <c r="F747" t="s">
+        <v>77</v>
+      </c>
+      <c r="G747" t="s">
         <v>101</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implement uncertainty for electrolyzers and PVS
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-PV-perovskite.xlsx
+++ b/premise/data/additional_inventories/lci-PV-perovskite.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A1A6DFD-11CE-924A-B007-63DA97BCF8DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57078C70-C97C-484D-9C3D-3D995785D4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2858" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2864" uniqueCount="459">
   <si>
     <t>Database</t>
   </si>
@@ -977,12 +977,6 @@
     <t>B11</t>
   </si>
   <si>
-    <t>perovskite module assembly</t>
-  </si>
-  <si>
-    <t>assembled perovskite cell</t>
-  </si>
-  <si>
     <t>Original activity in GaBi: Aluminium frame profile, powder coated (EN15804 A1-A3)</t>
   </si>
   <si>
@@ -1361,9 +1355,6 @@
     <t>stockpiling of anode slime from electrorefining of copper, anode</t>
   </si>
   <si>
-    <t>Data from Table 1. Cells per module: 72 | Gross module are: 2 square meter | Performance. Yield over lifetime: 11500 kWh/per module (each module 2 square meter)</t>
-  </si>
-  <si>
     <t>market for t-butyl amine</t>
   </si>
   <si>
@@ -1397,19 +1388,50 @@
     <t>electricity production, photovoltaic, 0.5kWp, perovskite-on-silicon tandem</t>
   </si>
   <si>
-    <t>photovoltaic panel production, 0.5kWp, perovskite</t>
-  </si>
-  <si>
     <t>market for metal part of electronics scrap, in copper, anode</t>
+  </si>
+  <si>
+    <t>uncertainty type</t>
+  </si>
+  <si>
+    <t>loc</t>
+  </si>
+  <si>
+    <t>minimum</t>
+  </si>
+  <si>
+    <t>maximum</t>
+  </si>
+  <si>
+    <t>Data from Table 1. Cells per module: 72 | Gross module are: 2 square meter | Performance. Yield over lifetime: 11500 kWh/per module (each module occupies 2 square meter)</t>
+  </si>
+  <si>
+    <t>2 m2/500Wp</t>
+  </si>
+  <si>
+    <t>photovoltaic panel installation, 0.5kWp, perovskite</t>
+  </si>
+  <si>
+    <t>perovskite photovoltaic module assembly</t>
+  </si>
+  <si>
+    <t>perovskite photovoltaic module</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1459,16 +1481,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1749,10 +1773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H747"/>
+  <dimension ref="A1:L747"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A497" zoomScale="78" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B535" sqref="B535"/>
+    <sheetView tabSelected="1" topLeftCell="A527" zoomScale="78" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D565" sqref="D565"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1764,6 +1788,7 @@
     <col min="5" max="5" width="26.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="78.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1915,7 +1940,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B14" s="4">
         <f>1830.1110288/35467268</f>
@@ -1931,7 +1956,7 @@
         <v>77</v>
       </c>
       <c r="G14" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
@@ -2260,7 +2285,7 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="B30" s="3">
         <f>59478608.436/35467268</f>
@@ -2276,7 +2301,7 @@
         <v>77</v>
       </c>
       <c r="G30" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -2933,7 +2958,7 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="B77">
         <f>428058757.128493/35422933.915</f>
@@ -2949,7 +2974,7 @@
         <v>77</v>
       </c>
       <c r="G77" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -3491,7 +3516,7 @@
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B109">
         <f>-3000/35367093.098703</f>
@@ -3512,7 +3537,7 @@
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="B110">
         <f>-5000/35367093.098703</f>
@@ -3578,7 +3603,7 @@
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B113">
         <f>-43830000/35367093.098703</f>
@@ -3594,7 +3619,7 @@
         <v>77</v>
       </c>
       <c r="G113" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H113" t="s">
         <v>211</v>
@@ -3602,7 +3627,7 @@
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B114">
         <f>-65745000/35367093.098703</f>
@@ -3618,7 +3643,7 @@
         <v>77</v>
       </c>
       <c r="G114" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H114" t="s">
         <v>211</v>
@@ -3626,7 +3651,7 @@
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B115">
         <f>-66621600/35367093.098703</f>
@@ -3642,7 +3667,7 @@
         <v>77</v>
       </c>
       <c r="G115" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H115" t="s">
         <v>211</v>
@@ -3929,7 +3954,7 @@
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B135">
         <f>46.5001236/35317005.6480545</f>
@@ -3945,10 +3970,10 @@
         <v>77</v>
       </c>
       <c r="G135" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H135" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -4541,7 +4566,7 @@
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B164">
         <f>30.6056124/35317005.6480545</f>
@@ -4557,7 +4582,7 @@
         <v>77</v>
       </c>
       <c r="G164" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.2">
@@ -4847,7 +4872,7 @@
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B178">
         <f>312.42024*0.08988/35317005.6480545</f>
@@ -4863,7 +4888,7 @@
         <v>77</v>
       </c>
       <c r="G178" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H178" s="6" t="s">
         <v>204</v>
@@ -4895,7 +4920,7 @@
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B180">
         <f>5259600*0.07078/35317005.6480545</f>
@@ -4911,7 +4936,7 @@
         <v>77</v>
       </c>
       <c r="G180" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H180" t="s">
         <v>203</v>
@@ -5075,7 +5100,7 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B188">
         <f>-(20161800+157788)/35317005.6480545</f>
@@ -5091,7 +5116,7 @@
         <v>77</v>
       </c>
       <c r="G188" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H188" t="s">
         <v>211</v>
@@ -5099,7 +5124,7 @@
     </row>
     <row r="189" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A189" s="5" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="B189">
         <f>-(157788)/35317005.6480545</f>
@@ -5115,7 +5140,7 @@
         <v>77</v>
       </c>
       <c r="G189" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="192" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -5483,7 +5508,7 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B213">
         <f>-1472688/35266918.197406</f>
@@ -5499,7 +5524,7 @@
         <v>77</v>
       </c>
       <c r="G213" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H213" t="s">
         <v>211</v>
@@ -5870,7 +5895,7 @@
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B237">
         <f>-1472688/35266918.197406</f>
@@ -5886,7 +5911,7 @@
         <v>77</v>
       </c>
       <c r="G237" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H237" t="s">
         <v>211</v>
@@ -6069,7 +6094,7 @@
         <v>77</v>
       </c>
       <c r="G252" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.2">
@@ -6111,7 +6136,7 @@
         <v>77</v>
       </c>
       <c r="G254" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.2">
@@ -6132,7 +6157,7 @@
         <v>77</v>
       </c>
       <c r="G255" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.2">
@@ -6153,7 +6178,7 @@
         <v>77</v>
       </c>
       <c r="G256" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.2">
@@ -6174,7 +6199,7 @@
         <v>77</v>
       </c>
       <c r="G257" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.2">
@@ -6195,7 +6220,7 @@
         <v>77</v>
       </c>
       <c r="G258" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.2">
@@ -6221,7 +6246,7 @@
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B260">
         <f>575.256965526288/35166743.2961089</f>
@@ -6237,7 +6262,7 @@
         <v>77</v>
       </c>
       <c r="G260" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.2">
@@ -6258,7 +6283,7 @@
         <v>77</v>
       </c>
       <c r="G261" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.2">
@@ -6279,7 +6304,7 @@
         <v>77</v>
       </c>
       <c r="G262" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.2">
@@ -6300,7 +6325,7 @@
         <v>77</v>
       </c>
       <c r="G263" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.2">
@@ -6326,7 +6351,7 @@
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B265">
         <f>2.87174093374893/35166743.2961089</f>
@@ -6342,7 +6367,7 @@
         <v>77</v>
       </c>
       <c r="G265" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.2">
@@ -6363,7 +6388,7 @@
         <v>77</v>
       </c>
       <c r="G266" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.2">
@@ -6405,7 +6430,7 @@
         <v>77</v>
       </c>
       <c r="G268" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.2">
@@ -6426,7 +6451,7 @@
         <v>77</v>
       </c>
       <c r="G269" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.2">
@@ -6447,7 +6472,7 @@
         <v>77</v>
       </c>
       <c r="G270" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.2">
@@ -6468,7 +6493,7 @@
         <v>77</v>
       </c>
       <c r="G271" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.2">
@@ -6489,7 +6514,7 @@
         <v>77</v>
       </c>
       <c r="G272" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.2">
@@ -6510,7 +6535,7 @@
         <v>77</v>
       </c>
       <c r="G273" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.2">
@@ -6552,7 +6577,7 @@
         <v>77</v>
       </c>
       <c r="G275" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.2">
@@ -6594,7 +6619,7 @@
         <v>77</v>
       </c>
       <c r="G277" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.2">
@@ -6636,7 +6661,7 @@
         <v>77</v>
       </c>
       <c r="G279" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.2">
@@ -6657,7 +6682,7 @@
         <v>77</v>
       </c>
       <c r="G280" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.2">
@@ -6678,7 +6703,7 @@
         <v>77</v>
       </c>
       <c r="G281" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.2">
@@ -6699,7 +6724,7 @@
         <v>77</v>
       </c>
       <c r="G282" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.2">
@@ -6756,7 +6781,7 @@
         <v>79</v>
       </c>
       <c r="E285" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F285" t="s">
         <v>77</v>
@@ -6783,7 +6808,7 @@
         <v>77</v>
       </c>
       <c r="G286" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.2">
@@ -6867,7 +6892,7 @@
         <v>77</v>
       </c>
       <c r="G290" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.2">
@@ -6888,7 +6913,7 @@
         <v>77</v>
       </c>
       <c r="G291" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.2">
@@ -6909,7 +6934,7 @@
         <v>77</v>
       </c>
       <c r="G292" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.2">
@@ -6951,12 +6976,12 @@
         <v>77</v>
       </c>
       <c r="G294" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="B295">
         <f>2381.0003944374/35166743.2961089</f>
@@ -6972,7 +6997,7 @@
         <v>77</v>
       </c>
       <c r="G295" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.2">
@@ -6998,7 +7023,7 @@
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B297">
         <f>-127.229028710395/35166743.2961089</f>
@@ -7014,7 +7039,7 @@
         <v>77</v>
       </c>
       <c r="G297" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.2">
@@ -7040,7 +7065,7 @@
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B299">
         <f>413.494343308785/35166743.2961089</f>
@@ -7056,7 +7081,7 @@
         <v>77</v>
       </c>
       <c r="G299" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.2">
@@ -7140,7 +7165,7 @@
         <v>77</v>
       </c>
       <c r="G303" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.2">
@@ -7161,7 +7186,7 @@
         <v>77</v>
       </c>
       <c r="G304" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.2">
@@ -7203,7 +7228,7 @@
         <v>77</v>
       </c>
       <c r="G306" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.2">
@@ -7224,7 +7249,7 @@
         <v>77</v>
       </c>
       <c r="G307" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.2">
@@ -7245,7 +7270,7 @@
         <v>77</v>
       </c>
       <c r="G308" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.2">
@@ -7271,7 +7296,7 @@
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="B310">
         <f>-127.960230024823/35166743.2961089</f>
@@ -7287,7 +7312,7 @@
         <v>77</v>
       </c>
       <c r="G310" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.2">
@@ -7313,7 +7338,7 @@
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="B312">
         <f>415.870747580675/35166743.2961089</f>
@@ -7329,7 +7354,7 @@
         <v>77</v>
       </c>
       <c r="G312" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.2">
@@ -7508,7 +7533,7 @@
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B321">
         <f>-14025600/35166743.2961089</f>
@@ -7524,7 +7549,7 @@
         <v>77</v>
       </c>
       <c r="G321" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H321" t="s">
         <v>211</v>
@@ -7715,7 +7740,7 @@
     </row>
     <row r="337" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="B337">
         <f>4.17324674571931/35116655.8454604</f>
@@ -7731,10 +7756,10 @@
         <v>77</v>
       </c>
       <c r="G337" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H337" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
     </row>
     <row r="338" spans="1:8" x14ac:dyDescent="0.2">
@@ -8004,7 +8029,7 @@
         <v>79</v>
       </c>
       <c r="E350" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="F350" t="s">
         <v>77</v>
@@ -8270,7 +8295,7 @@
     </row>
     <row r="363" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B363">
         <f>-(16594290.8653846+438300)/35116655.8454604</f>
@@ -8286,7 +8311,7 @@
         <v>77</v>
       </c>
       <c r="G363" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H363" t="s">
         <v>211</v>
@@ -8615,7 +8640,7 @@
     </row>
     <row r="385" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B385">
         <f>-87660/35066568.3948119</f>
@@ -8631,7 +8656,7 @@
         <v>77</v>
       </c>
       <c r="G385" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H385" t="s">
         <v>211</v>
@@ -8981,7 +9006,7 @@
     </row>
     <row r="408" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B408">
         <f>-438300/35016480.9441634</f>
@@ -8997,7 +9022,7 @@
         <v>77</v>
       </c>
       <c r="G408" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H408" t="s">
         <v>211</v>
@@ -9395,7 +9420,7 @@
     </row>
     <row r="433" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A433" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B433">
         <f>-2629800/34966393.4935149</f>
@@ -9411,7 +9436,7 @@
         <v>77</v>
       </c>
       <c r="G433" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H433" t="s">
         <v>211</v>
@@ -9875,7 +9900,7 @@
     </row>
     <row r="462" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A462" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="B462">
         <f>-200/34916306.0428664</f>
@@ -9891,7 +9916,7 @@
         <v>77</v>
       </c>
       <c r="G462" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
     </row>
     <row r="463" spans="1:8" x14ac:dyDescent="0.2">
@@ -9912,12 +9937,12 @@
         <v>77</v>
       </c>
       <c r="G463" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="464" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A464" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B464">
         <f>-28489500/34916306.0428664</f>
@@ -9933,7 +9958,7 @@
         <v>77</v>
       </c>
       <c r="G464" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H464" t="s">
         <v>211</v>
@@ -10166,7 +10191,7 @@
     </row>
     <row r="482" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A482" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B482">
         <f>-(43830000+5697900)/34866218.5922179</f>
@@ -10182,7 +10207,7 @@
         <v>77</v>
       </c>
       <c r="G482" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H482" t="s">
         <v>211</v>
@@ -10217,7 +10242,7 @@
         <v>1</v>
       </c>
       <c r="B486" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="487" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -10225,7 +10250,7 @@
         <v>2</v>
       </c>
       <c r="B487" s="5" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
     </row>
     <row r="488" spans="1:8" x14ac:dyDescent="0.2">
@@ -10249,7 +10274,7 @@
         <v>6</v>
       </c>
       <c r="B490" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="491" spans="1:8" x14ac:dyDescent="0.2">
@@ -10442,7 +10467,7 @@
         <v>1</v>
       </c>
       <c r="B502" s="2" t="s">
-        <v>312</v>
+        <v>457</v>
       </c>
     </row>
     <row r="503" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -10450,7 +10475,7 @@
         <v>2</v>
       </c>
       <c r="B503" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="504" spans="1:8" x14ac:dyDescent="0.2">
@@ -10474,7 +10499,7 @@
         <v>6</v>
       </c>
       <c r="B506" t="s">
-        <v>313</v>
+        <v>458</v>
       </c>
     </row>
     <row r="507" spans="1:8" x14ac:dyDescent="0.2">
@@ -10482,7 +10507,7 @@
         <v>7</v>
       </c>
       <c r="B507" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
     </row>
     <row r="508" spans="1:8" x14ac:dyDescent="0.2">
@@ -10533,14 +10558,14 @@
     <row r="511" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A511" t="str">
         <f>B502</f>
-        <v>perovskite module assembly</v>
+        <v>perovskite photovoltaic module assembly</v>
       </c>
       <c r="B511" s="3">
         <f>483538.053104108/483538.053104108</f>
         <v>1</v>
       </c>
       <c r="C511" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E511" t="str">
         <f>B504</f>
@@ -10549,18 +10574,16 @@
       <c r="F511" t="s">
         <v>14</v>
       </c>
-      <c r="G511" t="str">
-        <f>B506</f>
-        <v>assembled perovskite cell</v>
+      <c r="G511" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="512" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A512" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B512" s="3">
-        <f>34816131.1415694/483538.053104108</f>
-        <v>72.002877370384169</v>
+        <v>36.001438685192085</v>
       </c>
       <c r="C512" t="s">
         <v>7</v>
@@ -10572,7 +10595,7 @@
         <v>77</v>
       </c>
       <c r="G512" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="513" spans="1:8" x14ac:dyDescent="0.2">
@@ -10580,8 +10603,7 @@
         <v>307</v>
       </c>
       <c r="B513">
-        <f>1644029.38055394/50.7/483538.053104108</f>
-        <v>6.7061143984219793E-2</v>
+        <v>3.3530571992109896E-2</v>
       </c>
       <c r="C513" t="s">
         <v>47</v>
@@ -10596,16 +10618,15 @@
         <v>306</v>
       </c>
       <c r="H513" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
     </row>
     <row r="514" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A514" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B514">
-        <f>75098.8243368525/483538.053104108</f>
-        <v>0.15531109465894169</v>
+        <v>7.7655547329470845E-2</v>
       </c>
       <c r="C514" t="s">
         <v>79</v>
@@ -10617,19 +10638,18 @@
         <v>77</v>
       </c>
       <c r="G514" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="H514" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="515" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A515" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B515">
-        <f>75098.8243368525/483538.053104108</f>
-        <v>0.15531109465894169</v>
+        <v>7.7655547329470845E-2</v>
       </c>
       <c r="C515" t="s">
         <v>79</v>
@@ -10641,19 +10661,18 @@
         <v>77</v>
       </c>
       <c r="G515" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H515" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="516" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A516" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="B516">
-        <f>4833/483538.053104108</f>
-        <v>9.9950768486041612E-3</v>
+        <v>4.9975384243020806E-3</v>
       </c>
       <c r="C516" t="s">
         <v>79</v>
@@ -10665,19 +10684,18 @@
         <v>77</v>
       </c>
       <c r="G516" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="H516" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="517" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A517" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B517">
-        <f>4833/483538.053104108</f>
-        <v>9.9950768486041612E-3</v>
+        <v>4.9975384243020806E-3</v>
       </c>
       <c r="C517" t="s">
         <v>79</v>
@@ -10689,19 +10707,18 @@
         <v>77</v>
       </c>
       <c r="G517" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="H517" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="518" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A518" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B518">
-        <f>11000000/483538.053104108</f>
-        <v>22.748985171662689</v>
+        <v>11.374492585831344</v>
       </c>
       <c r="C518" t="s">
         <v>79</v>
@@ -10713,16 +10730,15 @@
         <v>77</v>
       </c>
       <c r="G518" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="519" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A519" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B519">
-        <f>37800/483538.053104108</f>
-        <v>7.8173785408077248E-2</v>
+        <v>3.9086892704038624E-2</v>
       </c>
       <c r="C519" t="s">
         <v>79</v>
@@ -10734,10 +10750,10 @@
         <v>77</v>
       </c>
       <c r="G519" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H519" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="520" spans="1:8" x14ac:dyDescent="0.2">
@@ -10745,8 +10761,7 @@
         <v>51</v>
       </c>
       <c r="B520">
-        <f>87731.687736/3.6/483538.053104108</f>
-        <v>5.0399163216949636E-2</v>
+        <v>2.5199581608474818E-2</v>
       </c>
       <c r="C520" t="s">
         <v>81</v>
@@ -10761,7 +10776,7 @@
         <v>52</v>
       </c>
       <c r="H520" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="521" spans="1:8" x14ac:dyDescent="0.2">
@@ -10769,8 +10784,7 @@
         <v>55</v>
       </c>
       <c r="B521">
-        <f>850.311/483538.053104108</f>
-        <v>1.7585193027546977E-3</v>
+        <v>8.7925965137734883E-4</v>
       </c>
       <c r="C521" t="s">
         <v>80</v>
@@ -10785,16 +10799,15 @@
         <v>56</v>
       </c>
       <c r="H521" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="522" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A522" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="B522">
-        <f>336/483538.053104108</f>
-        <v>6.9487809251624218E-4</v>
+        <v>3.4743904625812109E-4</v>
       </c>
       <c r="C522" t="s">
         <v>79</v>
@@ -10806,19 +10819,18 @@
         <v>77</v>
       </c>
       <c r="G522" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="H522" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="523" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A523" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B523">
-        <f>250000/483538.053104108</f>
-        <v>0.51702239026506114</v>
+        <v>0.25851119513253057</v>
       </c>
       <c r="C523" t="s">
         <v>79</v>
@@ -10830,16 +10842,15 @@
         <v>77</v>
       </c>
       <c r="G523" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="524" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A524" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="B524">
-        <f>177500/483538.053104108</f>
-        <v>0.36708589708819339</v>
+        <v>0.1835429485440967</v>
       </c>
       <c r="C524" t="s">
         <v>79</v>
@@ -10851,16 +10862,15 @@
         <v>77</v>
       </c>
       <c r="G524" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="525" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A525" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B525">
-        <f>27500/483538.053104108</f>
-        <v>5.6872462929156729E-2</v>
+        <v>2.8436231464578365E-2</v>
       </c>
       <c r="C525" t="s">
         <v>79</v>
@@ -10872,16 +10882,15 @@
         <v>77</v>
       </c>
       <c r="G525" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
     <row r="526" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A526" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="B526">
-        <f>45000/483538.053104108</f>
-        <v>9.306403024771101E-2</v>
+        <v>4.6532015123855505E-2</v>
       </c>
       <c r="C526" t="s">
         <v>79</v>
@@ -10893,16 +10902,15 @@
         <v>77</v>
       </c>
       <c r="G526" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
     </row>
     <row r="527" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A527" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B527">
-        <f>1500/483538.053104108</f>
-        <v>3.102134341590367E-3</v>
+        <v>1.5510671707951835E-3</v>
       </c>
       <c r="C527" t="s">
         <v>79</v>
@@ -10914,7 +10922,7 @@
         <v>77</v>
       </c>
       <c r="G527" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
     </row>
     <row r="528" spans="1:8" x14ac:dyDescent="0.2">
@@ -10922,8 +10930,7 @@
         <v>84</v>
       </c>
       <c r="B528">
-        <f>13000/483538.053104108</f>
-        <v>2.6885164293783178E-2</v>
+        <v>1.3442582146891589E-2</v>
       </c>
       <c r="C528" t="s">
         <v>79</v>
@@ -10940,11 +10947,10 @@
     </row>
     <row r="529" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A529" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="B529">
-        <f>75100/483538.053104108</f>
-        <v>0.15531352603562437</v>
+        <v>7.7656763017812186E-2</v>
       </c>
       <c r="C529" t="s">
         <v>79</v>
@@ -10956,10 +10962,10 @@
         <v>77</v>
       </c>
       <c r="G529" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H529" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="530" spans="1:8" x14ac:dyDescent="0.2">
@@ -10967,8 +10973,7 @@
         <v>51</v>
       </c>
       <c r="B530">
-        <f>387422.780617755/3.6/483538.053104108</f>
-        <v>0.22256250230903124</v>
+        <v>0.11128125115451562</v>
       </c>
       <c r="C530" t="s">
         <v>81</v>
@@ -10983,7 +10988,7 @@
         <v>52</v>
       </c>
       <c r="H530" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="531" spans="1:8" x14ac:dyDescent="0.2">
@@ -10991,8 +10996,7 @@
         <v>55</v>
       </c>
       <c r="B531">
-        <f>3755/483538.053104108</f>
-        <v>7.7656763017812181E-3</v>
+        <v>3.882838150890609E-3</v>
       </c>
       <c r="C531" t="s">
         <v>80</v>
@@ -11007,7 +11011,7 @@
         <v>56</v>
       </c>
       <c r="H531" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="532" spans="1:8" x14ac:dyDescent="0.2">
@@ -11015,8 +11019,7 @@
         <v>51</v>
       </c>
       <c r="B532">
-        <f>73639659.6/3.6/483538.053104108</f>
-        <v>42.303725360774941</v>
+        <v>21.15186268038747</v>
       </c>
       <c r="C532" t="s">
         <v>81</v>
@@ -11031,7 +11034,7 @@
         <v>52</v>
       </c>
       <c r="H532" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="533" spans="1:8" x14ac:dyDescent="0.2">
@@ -11039,8 +11042,7 @@
         <v>206</v>
       </c>
       <c r="B533">
-        <f>8795.30683506687/483538.053104108</f>
-        <v>1.818948225192361E-2</v>
+        <v>9.0947411259618052E-3</v>
       </c>
       <c r="C533" t="s">
         <v>133</v>
@@ -11063,8 +11065,7 @@
         <v>114</v>
       </c>
       <c r="B534">
-        <f>15088.024189726/483538.053104108</f>
-        <v>3.1203385323796795E-2</v>
+        <v>1.5601692661898398E-2</v>
       </c>
       <c r="C534" t="s">
         <v>133</v>
@@ -11084,11 +11085,10 @@
     </row>
     <row r="535" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A535" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="B535">
-        <f>5000/483538.053104108</f>
-        <v>1.0340447805301222E-2</v>
+        <v>5.1702239026506112E-3</v>
       </c>
       <c r="C535" t="s">
         <v>79</v>
@@ -11100,16 +11100,15 @@
         <v>77</v>
       </c>
       <c r="G535" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
     </row>
     <row r="536" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A536" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B536">
-        <f>-5000/483538.053104108</f>
-        <v>-1.0340447805301222E-2</v>
+        <v>-5.1702239026506112E-3</v>
       </c>
       <c r="C536" t="s">
         <v>79</v>
@@ -11121,7 +11120,7 @@
         <v>77</v>
       </c>
       <c r="G536" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
     </row>
     <row r="537" spans="1:8" x14ac:dyDescent="0.2">
@@ -11129,8 +11128,7 @@
         <v>95</v>
       </c>
       <c r="B537">
-        <f>-950/483538.053104108</f>
-        <v>-1.9646850830072325E-3</v>
+        <v>-9.8234254150361623E-4</v>
       </c>
       <c r="C537" t="s">
         <v>79</v>
@@ -11150,8 +11148,7 @@
         <v>130</v>
       </c>
       <c r="B538">
-        <f>-5/483538.053104108</f>
-        <v>-1.0340447805301223E-5</v>
+        <v>-5.1702239026506117E-6</v>
       </c>
       <c r="C538" t="s">
         <v>79</v>
@@ -11171,8 +11168,7 @@
         <v>206</v>
       </c>
       <c r="B539">
-        <f>-2198.82670876672/483538.053104108</f>
-        <v>-4.5473705629809087E-3</v>
+        <v>-2.2736852814904543E-3</v>
       </c>
       <c r="C539" t="s">
         <v>133</v>
@@ -11195,7 +11191,7 @@
         <v>1</v>
       </c>
       <c r="B542" s="2" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
     </row>
     <row r="543" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -11203,7 +11199,7 @@
         <v>2</v>
       </c>
       <c r="B543" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="544" spans="1:8" x14ac:dyDescent="0.2">
@@ -11227,7 +11223,7 @@
         <v>6</v>
       </c>
       <c r="B546" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
     </row>
     <row r="547" spans="1:8" x14ac:dyDescent="0.2">
@@ -11286,7 +11282,7 @@
     <row r="551" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A551" t="str">
         <f>B542</f>
-        <v>photovoltaic panel production, 0.5kWp, perovskite</v>
+        <v>photovoltaic panel installation, 0.5kWp, perovskite</v>
       </c>
       <c r="B551" s="3">
         <f>483538.053104108/483538.053104108</f>
@@ -11309,14 +11305,13 @@
     </row>
     <row r="552" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A552" t="s">
-        <v>312</v>
+        <v>457</v>
       </c>
       <c r="B552" s="3">
-        <f>483538.053104108/483538.053104108</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C552" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="E552" t="s">
         <v>92</v>
@@ -11325,12 +11320,15 @@
         <v>77</v>
       </c>
       <c r="G552" t="s">
-        <v>313</v>
+        <v>458</v>
+      </c>
+      <c r="H552" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="553" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A553" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B553">
         <f>24176.902655205/483538.053104108</f>
@@ -11346,12 +11344,12 @@
         <v>77</v>
       </c>
       <c r="G553" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="554" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A554" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B554">
         <f>589916.424787002/483538.053104108</f>
@@ -11367,7 +11365,7 @@
         <v>77</v>
       </c>
       <c r="G554" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="556" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -11375,15 +11373,15 @@
         <v>1</v>
       </c>
       <c r="B556" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="557" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A557" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B557" s="5" t="s">
-        <v>440</v>
+      <c r="B557" s="8" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="558" spans="1:8" x14ac:dyDescent="0.2">
@@ -11407,10 +11405,10 @@
         <v>6</v>
       </c>
       <c r="B560" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="561" spans="1:8" x14ac:dyDescent="0.2">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="561" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A561" t="s">
         <v>7</v>
       </c>
@@ -11418,7 +11416,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="562" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="562" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A562" t="s">
         <v>8</v>
       </c>
@@ -11426,7 +11424,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="563" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="563" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A563" s="1" t="s">
         <v>9</v>
       </c>
@@ -11437,7 +11435,7 @@
       <c r="F563" s="1"/>
       <c r="G563" s="1"/>
     </row>
-    <row r="564" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="564" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A564" s="1" t="s">
         <v>10</v>
       </c>
@@ -11462,8 +11460,20 @@
       <c r="H564" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="565" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I564" s="1" t="s">
+        <v>450</v>
+      </c>
+      <c r="J564" s="1" t="s">
+        <v>451</v>
+      </c>
+      <c r="K564" s="1" t="s">
+        <v>452</v>
+      </c>
+      <c r="L564" s="1" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="565" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A565" t="str">
         <f>B556</f>
         <v>electricity production, photovoltaic, 0.5kWp, perovskite-on-silicon tandem</v>
@@ -11488,12 +11498,12 @@
         <v>electricity production, photovoltaic, 0.5kWp, perovskite-on-silicon tandem</v>
       </c>
     </row>
-    <row r="566" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="566" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A566" t="s">
-        <v>452</v>
+        <v>456</v>
       </c>
       <c r="B566" s="4">
-        <f>1/(11500)</f>
+        <f>1/(25*460)</f>
         <v>8.6956521739130441E-5</v>
       </c>
       <c r="C566" t="s">
@@ -11506,26 +11516,41 @@
         <v>77</v>
       </c>
       <c r="G566" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="568" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>348</v>
+      </c>
+      <c r="I566" s="7">
+        <v>5</v>
+      </c>
+      <c r="J566" s="4">
+        <f>B566</f>
+        <v>8.6956521739130441E-5</v>
+      </c>
+      <c r="K566">
+        <f>1/(30*460)</f>
+        <v>7.2463768115942027E-5</v>
+      </c>
+      <c r="L566">
+        <f>1/(20*460)</f>
+        <v>1.0869565217391305E-4</v>
+      </c>
+    </row>
+    <row r="568" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A568" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B568" s="2" t="s">
-        <v>377</v>
-      </c>
-    </row>
-    <row r="569" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="569" spans="1:12" ht="16" x14ac:dyDescent="0.2">
       <c r="A569" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B569" s="5" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="570" spans="1:8" x14ac:dyDescent="0.2">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="570" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A570" t="s">
         <v>3</v>
       </c>
@@ -11533,7 +11558,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="571" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="571" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A571" t="s">
         <v>5</v>
       </c>
@@ -11541,15 +11566,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="572" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="572" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A572" t="s">
         <v>6</v>
       </c>
       <c r="B572" t="s">
-        <v>379</v>
-      </c>
-    </row>
-    <row r="573" spans="1:8" x14ac:dyDescent="0.2">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="573" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A573" t="s">
         <v>7</v>
       </c>
@@ -11557,7 +11582,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="574" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="574" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A574" t="s">
         <v>8</v>
       </c>
@@ -11565,7 +11590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="575" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="575" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A575" s="1" t="s">
         <v>9</v>
       </c>
@@ -11576,7 +11601,7 @@
       <c r="F575" s="1"/>
       <c r="G575" s="1"/>
     </row>
-    <row r="576" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="576" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A576" s="1" t="s">
         <v>10</v>
       </c>
@@ -11627,7 +11652,7 @@
         <v>abated exhaust</v>
       </c>
       <c r="H577" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="578" spans="1:8" x14ac:dyDescent="0.2">
@@ -11691,7 +11716,7 @@
         <v>52</v>
       </c>
       <c r="H580" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="581" spans="1:8" x14ac:dyDescent="0.2">
@@ -11719,7 +11744,7 @@
     </row>
     <row r="582" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A582" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="B582">
         <v>0.23200000000000001</v>
@@ -11734,10 +11759,10 @@
         <v>77</v>
       </c>
       <c r="G582" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H582" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="583" spans="1:8" x14ac:dyDescent="0.2">
@@ -11765,7 +11790,7 @@
     </row>
     <row r="584" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A584" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B584">
         <v>0</v>
@@ -11780,12 +11805,12 @@
         <v>78</v>
       </c>
       <c r="H584" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="585" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A585" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="B585">
         <v>0</v>
@@ -11800,12 +11825,12 @@
         <v>78</v>
       </c>
       <c r="H585" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="586" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A586" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B586">
         <v>0</v>
@@ -11820,12 +11845,12 @@
         <v>78</v>
       </c>
       <c r="H586" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
     </row>
     <row r="587" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A587" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="B587">
         <v>0</v>
@@ -11840,7 +11865,7 @@
         <v>78</v>
       </c>
       <c r="H587" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
     </row>
     <row r="590" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -11964,7 +11989,7 @@
     </row>
     <row r="600" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A600" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B600">
         <f>2.10977682373547E-07/0.7</f>
@@ -11980,10 +12005,10 @@
         <v>77</v>
       </c>
       <c r="G600" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="H600" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="601" spans="1:8" x14ac:dyDescent="0.2">
@@ -12028,12 +12053,12 @@
         <v>52</v>
       </c>
       <c r="H602" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="603" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A603" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B603">
         <f>3.97134460938441E-06*1000</f>
@@ -12078,7 +12103,7 @@
     </row>
     <row r="605" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A605" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B605">
         <f>-2.48209038086526E-06</f>
@@ -12094,12 +12119,12 @@
         <v>77</v>
       </c>
       <c r="G605" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="606" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A606" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B606">
         <f>-0.148925422851915</f>
@@ -12115,7 +12140,7 @@
         <v>77</v>
       </c>
       <c r="G606" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H606" t="s">
         <v>211</v>
@@ -12261,12 +12286,12 @@
         <v>52</v>
       </c>
       <c r="H619" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="620" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A620" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B620">
         <f>3.63854545454545*1000/2307.27272727273</f>
@@ -12314,7 +12339,7 @@
     </row>
     <row r="622" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A622" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B622">
         <f>3.27272727272727E-07/2307.27272727273</f>
@@ -12330,7 +12355,7 @@
         <v>77</v>
       </c>
       <c r="G622" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="623" spans="1:8" x14ac:dyDescent="0.2">
@@ -12354,7 +12379,7 @@
         <v>253</v>
       </c>
       <c r="H623" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="626" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -12498,7 +12523,7 @@
         <v>105</v>
       </c>
       <c r="H636" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="637" spans="1:8" x14ac:dyDescent="0.2">
@@ -12542,12 +12567,12 @@
         <v>111</v>
       </c>
       <c r="H638" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="639" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A639" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="B639">
         <v>0.45705279747832939</v>
@@ -12562,12 +12587,12 @@
         <v>77</v>
       </c>
       <c r="G639" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="640" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A640" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B640">
         <v>0.33884948778565799</v>
@@ -12582,12 +12607,12 @@
         <v>77</v>
       </c>
       <c r="G640" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="641" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A641" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B641">
         <v>0.42111899133175729</v>
@@ -12602,7 +12627,7 @@
         <v>77</v>
       </c>
       <c r="G641" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="642" spans="1:8" x14ac:dyDescent="0.2">
@@ -12626,7 +12651,7 @@
         <v>52</v>
       </c>
       <c r="H642" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="643" spans="1:8" x14ac:dyDescent="0.2">
@@ -12655,7 +12680,7 @@
     </row>
     <row r="644" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A644" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B644">
         <v>315.20882584712399</v>
@@ -12696,12 +12721,12 @@
         <v>253</v>
       </c>
       <c r="H645" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="646" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A646" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B646">
         <f>-0.179790569157611*1000</f>
@@ -12717,12 +12742,12 @@
         <v>77</v>
       </c>
       <c r="G646" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="647" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A647" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="B647">
         <f>-78.8022064617809</f>
@@ -12738,7 +12763,7 @@
         <v>77</v>
       </c>
       <c r="G647" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H647" t="s">
         <v>211</v>
@@ -12746,7 +12771,7 @@
     </row>
     <row r="648" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A648" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B648">
         <v>-47.281323877068601</v>
@@ -12761,7 +12786,7 @@
         <v>77</v>
       </c>
       <c r="G648" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H648" t="s">
         <v>211</v>
@@ -12906,7 +12931,7 @@
         <v>253</v>
       </c>
       <c r="H661" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="662" spans="1:8" x14ac:dyDescent="0.2">
@@ -12932,7 +12957,7 @@
     </row>
     <row r="663" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A663" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B663">
         <v>1000</v>
@@ -13194,7 +13219,7 @@
     </row>
     <row r="687" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A687" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="B687">
         <v>1</v>
@@ -13209,10 +13234,10 @@
         <v>77</v>
       </c>
       <c r="G687" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H687" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="690" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -13220,7 +13245,7 @@
         <v>1</v>
       </c>
       <c r="B690" s="1" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
     </row>
     <row r="691" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -13252,7 +13277,7 @@
         <v>6</v>
       </c>
       <c r="B694" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
     </row>
     <row r="695" spans="1:8" x14ac:dyDescent="0.2">
@@ -13336,7 +13361,7 @@
     </row>
     <row r="700" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A700" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B700">
         <v>7.6051410753669521E-7</v>
@@ -13351,12 +13376,12 @@
         <v>77</v>
       </c>
       <c r="G700" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="701" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A701" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B701">
         <v>7.6051410753669521E-7</v>
@@ -13371,7 +13396,7 @@
         <v>77</v>
       </c>
       <c r="G701" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="702" spans="1:8" x14ac:dyDescent="0.2">
@@ -13397,7 +13422,7 @@
     </row>
     <row r="703" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A703" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B703">
         <v>1.1407711613050422E-5</v>
@@ -13412,7 +13437,7 @@
         <v>78</v>
       </c>
       <c r="H703" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="704" spans="1:8" x14ac:dyDescent="0.2">
@@ -13432,7 +13457,7 @@
         <v>78</v>
       </c>
       <c r="H704" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="705" spans="1:8" x14ac:dyDescent="0.2">
@@ -13452,7 +13477,7 @@
         <v>78</v>
       </c>
       <c r="H705" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="708" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -13460,7 +13485,7 @@
         <v>1</v>
       </c>
       <c r="B708" s="1" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="709" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -13492,7 +13517,7 @@
         <v>6</v>
       </c>
       <c r="B712" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="713" spans="1:8" x14ac:dyDescent="0.2">
@@ -13576,7 +13601,7 @@
     </row>
     <row r="718" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A718" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B718">
         <v>7.6051410753669521E-7</v>
@@ -13591,12 +13616,12 @@
         <v>77</v>
       </c>
       <c r="G718" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="719" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A719" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B719">
         <v>7.6051410753669521E-7</v>
@@ -13611,7 +13636,7 @@
         <v>77</v>
       </c>
       <c r="G719" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="720" spans="1:8" x14ac:dyDescent="0.2">
@@ -13637,7 +13662,7 @@
     </row>
     <row r="721" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A721" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B721">
         <v>1.1407711613050422E-5</v>
@@ -13652,7 +13677,7 @@
         <v>78</v>
       </c>
       <c r="H721" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="722" spans="1:8" x14ac:dyDescent="0.2">
@@ -13672,7 +13697,7 @@
         <v>78</v>
       </c>
       <c r="H722" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="723" spans="1:8" x14ac:dyDescent="0.2">
@@ -13692,7 +13717,7 @@
         <v>78</v>
       </c>
       <c r="H723" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="724" spans="1:8" x14ac:dyDescent="0.2">
@@ -13716,7 +13741,7 @@
         <v>111</v>
       </c>
       <c r="H724" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="725" spans="1:8" x14ac:dyDescent="0.2">
@@ -13765,7 +13790,7 @@
         <v>1</v>
       </c>
       <c r="B729" s="1" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
     </row>
     <row r="730" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -13797,7 +13822,7 @@
         <v>6</v>
       </c>
       <c r="B733" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="734" spans="1:8" x14ac:dyDescent="0.2">
@@ -13881,7 +13906,7 @@
     </row>
     <row r="739" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A739" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B739">
         <v>7.6051410753669521E-7</v>
@@ -13896,12 +13921,12 @@
         <v>77</v>
       </c>
       <c r="G739" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="740" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A740" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="B740">
         <v>7.6051410753669521E-7</v>
@@ -13916,7 +13941,7 @@
         <v>77</v>
       </c>
       <c r="G740" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
     </row>
     <row r="741" spans="1:8" x14ac:dyDescent="0.2">
@@ -13942,7 +13967,7 @@
     </row>
     <row r="742" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A742" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="B742">
         <v>1.1407711613050422E-5</v>
@@ -13957,7 +13982,7 @@
         <v>78</v>
       </c>
       <c r="H742" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="743" spans="1:8" x14ac:dyDescent="0.2">
@@ -13977,7 +14002,7 @@
         <v>78</v>
       </c>
       <c r="H743" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="744" spans="1:8" x14ac:dyDescent="0.2">
@@ -13997,7 +14022,7 @@
         <v>78</v>
       </c>
       <c r="H744" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="745" spans="1:8" x14ac:dyDescent="0.2">
@@ -14018,10 +14043,10 @@
         <v>77</v>
       </c>
       <c r="G745" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H745" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
     </row>
     <row r="746" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix unlinked exchanges with ei consequential 3.8/3.9
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-PV-perovskite.xlsx
+++ b/premise/data/additional_inventories/lci-PV-perovskite.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise/premise/data/additional_inventories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05468028-B5E8-EA4C-B4D7-4B8ED2EA91B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BAE77C-38CC-B748-90A0-DBA3BF4E3CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1777,7 +1777,7 @@
   <dimension ref="A1:L747"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D565" sqref="D565"/>
+      <selection activeCell="E748" sqref="E748"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4028,7 +4028,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>149</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>79</v>
       </c>
       <c r="E138" t="s">
-        <v>92</v>
+        <v>57</v>
       </c>
       <c r="F138" t="s">
         <v>77</v>
@@ -4724,7 +4724,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>194</v>
       </c>
@@ -6335,7 +6335,7 @@
         <v>79</v>
       </c>
       <c r="E263" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F263" t="s">
         <v>77</v>
@@ -14146,7 +14146,7 @@
   <autoFilter ref="A1:H747" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="treatment of wastewater from wafer fabrication, wastewater treatment"/>
+        <filter val="market for silicon tetrachloride"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>